<commit_message>
Done-gui7.3, 7.4- Tuấn làm countdown 7.3 nhé
</commit_message>
<xml_diff>
--- a/src/main/java/data/QuizTestAppData.xlsx
+++ b/src/main/java/data/QuizTestAppData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\btl oop\quiz-test-app\src\main\java\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\JavaProjects\QuizApp\quiz-test-app\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A7AB38-2BC6-4487-9069-4BEB660B8D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC596134-E12A-4E2F-85FC-2ACB5E722993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionBank" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="141">
   <si>
     <t>10-6-2023 12-00-00</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>root/Course : IT/OOP/GK</t>
-  </si>
-  <si>
-    <t>root/Course : Junior high school/Sinh học 7/CK</t>
   </si>
   <si>
     <t>Quá trình tiêu hóa thức ăn diễn ra chủ yếu ở đâu trong cơ thể người?</t>
@@ -349,24 +346,260 @@
 D. Tiêu hóa</t>
   </si>
   <si>
-    <t>Các tế bào gốc làm gì?</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>A. Tiêu hóa thức ăn
-B. Tạo ra hormone
-C. Tái tạo và phục hồi các tế bào khác
-D. Phát triển cơ bắp
-E. Làm cơ thể tồn tại</t>
-  </si>
-  <si>
-    <t>A. Cá
-B. Chim
-C. Rắn
-D. Rùa
-E. Sò</t>
+    <t>thang huy co ny chua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A. khong
+B. Ko
+C.KHum
+null
+null
+null
+null
+null
+null
+null</t>
+  </si>
+  <si>
+    <t>Biển lớn nhất trên Trái Đất là:</t>
+  </si>
+  <si>
+    <t>A. Thái Bình Dương
+B. Ấn Độ Dương
+C. Đại Tây Dương</t>
+  </si>
+  <si>
+    <t>Dòng sông lớn nhất châu Á là:</t>
+  </si>
+  <si>
+    <t>A. Sông Nile
+B. Sông Mekong
+C. Sông Dương Tử</t>
+  </si>
+  <si>
+    <t>Dãy núi cao nhất thế giới là:</t>
+  </si>
+  <si>
+    <t>A. Dãy Andes
+B. Dãy Himalaya
+C. Dãy Alps</t>
+  </si>
+  <si>
+    <t>Hòn đảo lớn nhất trên Trái Đất là:</t>
+  </si>
+  <si>
+    <t>A. Đảo Borneo
+B. Đảo Madagascar
+C. Đảo Greenland</t>
+  </si>
+  <si>
+    <t>Đảo lớn nhất của Việt Nam là:</t>
+  </si>
+  <si>
+    <t>A. Phú Quốc
+B. Cát Bà
+C. Hòn Tre</t>
+  </si>
+  <si>
+    <t>Châu lục có dân số đông nhất là:</t>
+  </si>
+  <si>
+    <t>A. Châu Á
+B. Châu Âu
+C. Châu Phi</t>
+  </si>
+  <si>
+    <t>Thành phố có dân số đông nhất thế giới là:</t>
+  </si>
+  <si>
+    <t>A. Tokyo
+B. New York
+C. Delhi</t>
+  </si>
+  <si>
+    <t>Núi cao nhất thế giới là:</t>
+  </si>
+  <si>
+    <t>A. Everest
+B. K2
+C. Kangchenjunga</t>
+  </si>
+  <si>
+    <t>Quốc gia nào là nơi sinh sống của người Eskimo?</t>
+  </si>
+  <si>
+    <t>A. Canada
+B. Greenland
+C. Alaska</t>
+  </si>
+  <si>
+    <t>Thành phố Paris nằm ở nước nào?</t>
+  </si>
+  <si>
+    <t>A. Pháp
+B. Ý
+C. Anh</t>
+  </si>
+  <si>
+    <t>Dòng sông Nile chảy qua bao nhiêu quốc gia?</t>
+  </si>
+  <si>
+    <t>A. 1
+B. 2
+C. 3</t>
+  </si>
+  <si>
+    <t>Quốc gia nào được gọi là "đất nụ cười"?</t>
+  </si>
+  <si>
+    <t>A. Brazil
+B. Ý
+C. Thái Lan</t>
+  </si>
+  <si>
+    <t>Dãy núi Andes nằm ở:</t>
+  </si>
+  <si>
+    <t>A. Nam Mỹ
+B. Bắc Mỹ
+C. Châu Âu</t>
+  </si>
+  <si>
+    <t>Thành phố nổi tiếng với ngọn núi Phật Di Lặc là:</t>
+  </si>
+  <si>
+    <t>A. Tokyo
+B. Kathmandu
+C. Hong Kong</t>
+  </si>
+  <si>
+    <t>Kênh đào nổi tiếng nằm ở Ai Cập là:</t>
+  </si>
+  <si>
+    <t>A. Kênh Panama
+B. Kênh Suez
+C. Kênh Kiel</t>
+  </si>
+  <si>
+    <t>Nước nào là quốc gia lớn nhất thế giới về diện tích?</t>
+  </si>
+  <si>
+    <t>A. Nga
+B. Trung Quốc
+C. Mỹ</t>
+  </si>
+  <si>
+    <t>Đại ngàn nổi tiếng của Việt Nam là:</t>
+  </si>
+  <si>
+    <t>A. Đại Sơn
+B. Trường Sơn
+C. Trường Giang</t>
+  </si>
+  <si>
+    <t>Kỳ quan thế giới Machu Picchu nằm ở quốc gia nào?</t>
+  </si>
+  <si>
+    <t>A. Peru
+B. Brazil
+C. Colombia</t>
+  </si>
+  <si>
+    <t>Địa danh nổi tiếng "Vịnh Hạ Long" nằm ở tỉnh nào của Việt Nam?</t>
+  </si>
+  <si>
+    <t>A. Quảng Ninh
+B. Thanh Hóa
+C. Nghệ An</t>
+  </si>
+  <si>
+    <t>Hệ thống sông Mê Kông chảy qua bao nhiêu quốc gia?</t>
+  </si>
+  <si>
+    <t>A. 2
+B. 4
+C. 6</t>
+  </si>
+  <si>
+    <t>Thành phố Moscow nằm ở quốc gia nào?</t>
+  </si>
+  <si>
+    <t>A. Nga
+B. Pháp
+C. Đức</t>
+  </si>
+  <si>
+    <t>Đảo Jeju nằm ở quốc gia nào?</t>
+  </si>
+  <si>
+    <t>A. Nhật Bản
+B. Hàn Quốc
+C. Indonesia</t>
+  </si>
+  <si>
+    <t>Dãy núi Alps nằm ở:</t>
+  </si>
+  <si>
+    <t>A. Châu Phi
+B. Châu Mỹ
+C. Châu Âu</t>
+  </si>
+  <si>
+    <t>Quốc gia nào là quê hương của người Maori?</t>
+  </si>
+  <si>
+    <t>A. Úc
+B. New Zealand
+C. Hawaii</t>
+  </si>
+  <si>
+    <t>Quốc gia nào là quê hương của kim cương?</t>
+  </si>
+  <si>
+    <t>A. Nam Phi
+B. Nga
+C. Ấn Độ</t>
+  </si>
+  <si>
+    <t>Thành phố nào được gọi là "thành phố của tình yêu"?</t>
+  </si>
+  <si>
+    <t>A. Paris
+B. Rome
+C. Barcelona</t>
+  </si>
+  <si>
+    <t>Đại dương nằm giữa châu lục Mỹ và châu lục châu Á là:</t>
+  </si>
+  <si>
+    <t>A. Đại Tây Dương
+B. Ấn Độ Dương
+C. Thái Bình Dương</t>
+  </si>
+  <si>
+    <t>Quốc gia nào nằm ở khu vực Châu Phi?</t>
+  </si>
+  <si>
+    <t>A. Argentina
+B. Nigeria
+C. Thụy Điển</t>
+  </si>
+  <si>
+    <t>Kênh đào Panama nằm ở đất nước nào?</t>
+  </si>
+  <si>
+    <t>A. Mexico
+B. Panama
+C. Colombia</t>
+  </si>
+  <si>
+    <t>Thành phố Sydney nằm ở quốc gia nào?</t>
+  </si>
+  <si>
+    <t>A. Úc
+B. New Zealand
+C. Canada</t>
   </si>
 </sst>
 </file>
@@ -685,367 +918,808 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="94.5546875"/>
+    <col min="2" max="2" customWidth="true" width="101.5546875"/>
+    <col min="3" max="3" customWidth="true" width="5.21875"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>28</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>37</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>19</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>82</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s" s="0">
         <v>42</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s" s="0">
         <v>44</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>46</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>47</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>48</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>49</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s" s="0">
         <v>50</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s" s="0">
         <v>52</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s" s="0">
         <v>54</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s" s="0">
         <v>56</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>57</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s" s="0">
         <v>58</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s" s="0">
         <v>60</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>61</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s" s="0">
         <v>62</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s" s="0">
         <v>64</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>65</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>19</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s" s="0">
         <v>67</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s" s="0">
-        <v>68</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s" s="0">
         <v>69</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s" s="0">
-        <v>70</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s" s="0">
         <v>71</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s" s="0">
-        <v>72</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s" s="0">
         <v>73</v>
-      </c>
-      <c r="B22" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D22" t="s" s="0">
-        <v>83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s" s="0">
         <v>75</v>
-      </c>
-      <c r="B23" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s" s="0">
-        <v>76</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>19</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s" s="0">
         <v>78</v>
-      </c>
-      <c r="B25" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s" s="0">
-        <v>79</v>
       </c>
     </row>
     <row r="26"/>
     <row r="27"/>
     <row r="28"/>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60"/>
+    <row r="61"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1053,26 +1727,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7375D0D9-A088-4E33-84C0-F60360358F66}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="66.26953125"/>
+    <col min="1" max="1" customWidth="true" width="66.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
         <v>8</v>
       </c>
       <c r="B1" s="0" t="n">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>61.0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
         <v>9</v>
       </c>
@@ -1080,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
@@ -1088,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
         <v>11</v>
       </c>
@@ -1096,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
@@ -1104,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s" s="0">
         <v>13</v>
       </c>
@@ -1112,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s" s="0">
         <v>14</v>
       </c>
@@ -1120,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s" s="0">
         <v>15</v>
       </c>
@@ -1128,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s" s="0">
         <v>16</v>
       </c>
@@ -1136,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s" s="0">
         <v>17</v>
       </c>
@@ -1144,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s" s="0">
         <v>18</v>
       </c>
@@ -1152,31 +1826,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s" s="0">
         <v>22</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>61.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s" s="0">
         <v>19</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B14" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="0" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s" s="0">
         <v>21</v>
       </c>
@@ -1184,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s" s="0">
         <v>23</v>
       </c>
@@ -1192,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s" s="0">
         <v>24</v>
       </c>
@@ -1200,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s" s="0">
         <v>25</v>
       </c>
@@ -1208,19 +1882,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s" s="0">
         <v>26</v>
       </c>
       <c r="B19" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B20" s="0">
         <v>0</v>
       </c>
     </row>
@@ -1237,15 +1903,15 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.54296875"/>
-    <col min="2" max="2" customWidth="true" width="19.26953125"/>
-    <col min="3" max="3" customWidth="true" width="17.453125"/>
-    <col min="5" max="5" customWidth="true" width="38.7265625"/>
+    <col min="1" max="1" customWidth="true" width="35.5546875"/>
+    <col min="2" max="2" customWidth="true" width="19.21875"/>
+    <col min="3" max="3" customWidth="true" width="17.44140625"/>
+    <col min="5" max="5" customWidth="true" width="38.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
         <v>3</v>
       </c>
@@ -1262,7 +1928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
@@ -1279,7 +1945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s" s="0">
         <v>3</v>
       </c>
@@ -1296,7 +1962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s" s="0">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Function for GUI 6.3, 6.4
</commit_message>
<xml_diff>
--- a/src/main/java/data/QuizTestAppData.xlsx
+++ b/src/main/java/data/QuizTestAppData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\btl oop\quiz-test-app\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3061E72-3467-4D86-BF6F-59D0B6BDCC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4840A02C-1321-443D-9825-342F98DCAFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="284">
   <si>
     <t>10-6-2023 12-00-00</t>
   </si>
@@ -940,6 +940,257 @@
     <t>A. Úc
 B. New Zealand
 C. Canada</t>
+  </si>
+  <si>
+    <t>Thi gi do</t>
+  </si>
+  <si>
+    <t>10/9/2023</t>
+  </si>
+  <si>
+    <t>11/9/2023</t>
+  </si>
+  <si>
+    <t>1, 4, 7, 9</t>
+  </si>
+  <si>
+    <t>Đơn vị đo dung lượng bộ nhớ được sử dụng trong máy tính là:</t>
+  </si>
+  <si>
+    <t>A. Byte
+B. Bit
+C. Kilobyte</t>
+  </si>
+  <si>
+    <t>Đâu là phần mềm văn bản phổ biến nhất?</t>
+  </si>
+  <si>
+    <t>A. Microsoft Word
+B. Adobe Photoshop
+C. Google Chrome</t>
+  </si>
+  <si>
+    <t>Loại màn hình nào có khả năng hiển thị hình ảnh chất lượng cao nhất?</t>
+  </si>
+  <si>
+    <t>A. LCD
+B. LED
+C. OLED</t>
+  </si>
+  <si>
+    <t>Thiết bị nào dùng để lưu trữ dữ liệu lâu dài và có khả năng di động?</t>
+  </si>
+  <si>
+    <t>A. USB
+B. CD/DVD
+C. Ổ cứng di động</t>
+  </si>
+  <si>
+    <t>Giao thức truyền thông phổ biến trong mạng Internet là:</t>
+  </si>
+  <si>
+    <t>A. HTTP
+B. FTP
+C. SMTP</t>
+  </si>
+  <si>
+    <t>Đâu không phải là phần cứng của máy tính?</t>
+  </si>
+  <si>
+    <t>A. Bàn phím
+B. Hệ điều hành
+C. Chuột</t>
+  </si>
+  <si>
+    <t>Định dạng file hình ảnh phổ biến là:</t>
+  </si>
+  <si>
+    <t>A. JPG
+B. MP3
+C. PDF</t>
+  </si>
+  <si>
+    <t>Loại kết nối không dây phổ biến cho các thiết bị di động là:</t>
+  </si>
+  <si>
+    <t>A. Wi-Fi
+B. Bluetooth
+C. NFC</t>
+  </si>
+  <si>
+    <t>Giao diện nào được sử dụng phổ biến trong các thiết bị di động?</t>
+  </si>
+  <si>
+    <t>A. Touchscreen
+B. Keyboard
+C. Mouse</t>
+  </si>
+  <si>
+    <t>Công nghệ nào cho phép chuyển dữ liệu từ thiết bị di động sang máy tính một cách nhanh chóng và không cần dây?</t>
+  </si>
+  <si>
+    <t>A. Bluetooth
+B. Wi-Fi
+C. NFC</t>
+  </si>
+  <si>
+    <t>Loại pin nào được sử dụng phổ biến trong các thiết bị di động?</t>
+  </si>
+  <si>
+    <t>A. Pin kiềm
+B. Pin lithium-ion
+C. Pin axit chì</t>
+  </si>
+  <si>
+    <t>Loại máy tính nào có kích thước nhỏ gọn, dễ dàng mang theo?</t>
+  </si>
+  <si>
+    <t>A. Máy tính xách tay
+B. Máy tính để bàn
+C. Máy tính siêu việt</t>
+  </si>
+  <si>
+    <t>Đâu là trình duyệt web phổ biến nhất?</t>
+  </si>
+  <si>
+    <t>A. Google Chrome
+B. Safari
+C. Mozilla Firefox</t>
+  </si>
+  <si>
+    <t>Loại kết nối dùng để truyền dữ liệu giữa máy tính và máy in là:</t>
+  </si>
+  <si>
+    <t>A. USB
+B. HDMI
+C. Ethernet</t>
+  </si>
+  <si>
+    <t>Loại kết nối dùng để truyền âm thanh và hình ảnh chất lượng cao từ máy tính ra TV là:</t>
+  </si>
+  <si>
+    <t>A. VGA
+B. HDMI
+C. DVI</t>
+  </si>
+  <si>
+    <t>Phần mềm nào được sử dụng để tạo bài thuyết trình?</t>
+  </si>
+  <si>
+    <t>A. Microsoft PowerPoint
+B. Adobe Illustrator
+C. Google Docs</t>
+  </si>
+  <si>
+    <t>Đơn vị đo tốc độ mạng là:</t>
+  </si>
+  <si>
+    <t>A. Kilobyte
+B. Megabyte
+C. Megabit</t>
+  </si>
+  <si>
+    <t>Loại máy tính nào được sử dụng phổ biến trong việc xử lý đồ họa và video?</t>
+  </si>
+  <si>
+    <t>A. Máy tính để bàn
+B. Máy tính xách tay
+C. Máy tính Workstation</t>
+  </si>
+  <si>
+    <t>Phần mềm nào được sử dụng để chỉnh sửa video chuyên nghiệp?</t>
+  </si>
+  <si>
+    <t>A. Adobe Premiere Pro
+B. Microsoft Word
+C. Windows Media Player</t>
+  </si>
+  <si>
+    <t>Loại màn hình nào được sử dụng phổ biến trong các thiết bị di động?</t>
+  </si>
+  <si>
+    <t>A. LCD
+B. AMOLED
+C. IPS</t>
+  </si>
+  <si>
+    <t>Loại ổ đĩa nào không dùng để lưu trữ dữ liệu trong máy tính?</t>
+  </si>
+  <si>
+    <t>A. Ổ cứng SSD
+B. Ổ đĩa CD/DVD
+C. Ổ đĩa RAM</t>
+  </si>
+  <si>
+    <t>Giao diện nào cho phép kết nối nhanh chóng và dễ dàng giữa các thiết bị điện tử?</t>
+  </si>
+  <si>
+    <t>A. USB
+B. Bluetooth
+C. HDMI</t>
+  </si>
+  <si>
+    <t>Phần mềm nào được sử dụng để xử lý và tính toán dữ liệu số lớn?</t>
+  </si>
+  <si>
+    <t>A. Microsoft Excel
+B. Adobe Photoshop
+C. Google Chrome</t>
+  </si>
+  <si>
+    <t>Công nghệ nào cho phép truyền tải dữ liệu không dây trong phạm vi gần?</t>
+  </si>
+  <si>
+    <t>A. Wi-Fi
+B. NFC
+C. Ethernet</t>
+  </si>
+  <si>
+    <t>Loại máy quét nào được sử dụng để chuyển đổi tài liệu giấy thành dạng số?</t>
+  </si>
+  <si>
+    <t>A. Máy quét phẳng
+B. Máy quét mã vạch
+C. Máy quét 3D</t>
+  </si>
+  <si>
+    <t>Phần mềm nào được sử dụng để duyệt và tìm kiếm thông tin trên Internet?</t>
+  </si>
+  <si>
+    <t>A. Google Chrome
+B. Microsoft Word
+C. Adobe Photoshop</t>
+  </si>
+  <si>
+    <t>Loại ứng dụng nào được sử dụng để giao tiếp và chia sẻ thông tin trong mạng xã hội?</t>
+  </si>
+  <si>
+    <t>A. Facebook
+B. Microsoft Excel
+C. Adobe Illustrator</t>
+  </si>
+  <si>
+    <t>ques for fun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. sbsbs
+B. snsksks
+null
+null
+null
+null
+null
+null
+null
+null
+</t>
+  </si>
+  <si>
+    <t>A. sbsbs
+B. snsksks</t>
+  </si>
+  <si>
+    <t>ques for fun abcdefxyz</t>
   </si>
 </sst>
 </file>
@@ -1258,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,7 +1536,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>32</v>
@@ -2064,7 +2315,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s" s="0">
         <v>114</v>
       </c>
@@ -2078,7 +2329,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
         <v>116</v>
       </c>
@@ -2092,7 +2343,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s" s="0">
         <v>118</v>
       </c>
@@ -2106,7 +2357,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
         <v>120</v>
       </c>
@@ -2120,7 +2371,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
         <v>122</v>
       </c>
@@ -2134,7 +2385,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
         <v>124</v>
       </c>
@@ -2148,7 +2399,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
         <v>126</v>
       </c>
@@ -2162,7 +2413,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
         <v>128</v>
       </c>
@@ -2176,7 +2427,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
         <v>130</v>
       </c>
@@ -2190,7 +2441,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
         <v>132</v>
       </c>
@@ -2204,7 +2455,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
         <v>134</v>
       </c>
@@ -2218,7 +2469,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s" s="0">
         <v>136</v>
       </c>
@@ -2232,7 +2483,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s" s="0">
         <v>138</v>
       </c>
@@ -2246,7 +2497,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s" s="0">
         <v>140</v>
       </c>
@@ -2260,7 +2511,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s" s="0">
         <v>142</v>
       </c>
@@ -2274,7 +2525,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s" s="0">
         <v>144</v>
       </c>
@@ -2288,7 +2539,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s" s="0">
         <v>146</v>
       </c>
@@ -2302,7 +2553,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s" s="0">
         <v>148</v>
       </c>
@@ -2316,7 +2567,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s" s="0">
         <v>149</v>
       </c>
@@ -2330,7 +2581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s" s="0">
         <v>151</v>
       </c>
@@ -2344,7 +2595,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s" s="0">
         <v>153</v>
       </c>
@@ -2358,7 +2609,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s" s="0">
         <v>155</v>
       </c>
@@ -2372,7 +2623,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s" s="0">
         <v>157</v>
       </c>
@@ -2386,7 +2637,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s" s="0">
         <v>159</v>
       </c>
@@ -2400,7 +2651,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s" s="0">
         <v>160</v>
       </c>
@@ -2414,10 +2665,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s" s="0">
         <v>162</v>
       </c>
@@ -2431,7 +2679,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s" s="0">
         <v>164</v>
       </c>
@@ -2445,7 +2693,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s" s="0">
         <v>166</v>
       </c>
@@ -2459,7 +2707,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s" s="0">
         <v>168</v>
       </c>
@@ -2473,7 +2721,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s" s="0">
         <v>170</v>
       </c>
@@ -2487,7 +2735,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s" s="0">
         <v>172</v>
       </c>
@@ -2501,7 +2749,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s" s="0">
         <v>174</v>
       </c>
@@ -2515,7 +2763,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s" s="0">
         <v>176</v>
       </c>
@@ -2529,7 +2777,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s" s="0">
         <v>178</v>
       </c>
@@ -2543,7 +2791,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s" s="0">
         <v>180</v>
       </c>
@@ -2557,7 +2805,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s" s="0">
         <v>182</v>
       </c>
@@ -2571,7 +2819,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s" s="0">
         <v>184</v>
       </c>
@@ -2585,7 +2833,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s" s="0">
         <v>186</v>
       </c>
@@ -2599,7 +2847,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s" s="0">
         <v>188</v>
       </c>
@@ -2613,7 +2861,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s" s="0">
         <v>190</v>
       </c>
@@ -2627,7 +2875,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s" s="0">
         <v>192</v>
       </c>
@@ -2641,7 +2889,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s" s="0">
         <v>194</v>
       </c>
@@ -2655,7 +2903,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s" s="0">
         <v>196</v>
       </c>
@@ -2669,7 +2917,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s" s="0">
         <v>198</v>
       </c>
@@ -2683,7 +2931,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s" s="0">
         <v>200</v>
       </c>
@@ -2697,7 +2945,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s" s="0">
         <v>202</v>
       </c>
@@ -2711,7 +2959,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s" s="0">
         <v>204</v>
       </c>
@@ -2725,7 +2973,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s" s="0">
         <v>206</v>
       </c>
@@ -2739,7 +2987,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s" s="0">
         <v>208</v>
       </c>
@@ -2753,7 +3001,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s" s="0">
         <v>210</v>
       </c>
@@ -2767,7 +3015,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s" s="0">
         <v>212</v>
       </c>
@@ -2781,7 +3029,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s" s="0">
         <v>214</v>
       </c>
@@ -2795,7 +3043,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s" s="0">
         <v>216</v>
       </c>
@@ -2809,7 +3057,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s" s="0">
         <v>218</v>
       </c>
@@ -2823,7 +3071,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s" s="0">
         <v>220</v>
       </c>
@@ -2837,8 +3085,412 @@
         <v>221</v>
       </c>
     </row>
-    <row r="116"/>
-    <row r="117"/>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="B116" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C116" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D116" t="s" s="0">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" t="s" s="0">
+        <v>228</v>
+      </c>
+      <c r="B117" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C117" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D117" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" t="s" s="0">
+        <v>230</v>
+      </c>
+      <c r="B118" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C118" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D118" t="s" s="0">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B119" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C119" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D119" t="s" s="0">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B120" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C120" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D120" t="s" s="0">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B121" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C121" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D121" t="s" s="0">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B122" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C122" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D122" t="s" s="0">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123" t="s" s="0">
+        <v>240</v>
+      </c>
+      <c r="B123" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C123" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D123" t="s" s="0">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124" t="s" s="0">
+        <v>242</v>
+      </c>
+      <c r="B124" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C124" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D124" t="s" s="0">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125" t="s" s="0">
+        <v>244</v>
+      </c>
+      <c r="B125" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C125" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D125" t="s" s="0">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126" t="s" s="0">
+        <v>246</v>
+      </c>
+      <c r="B126" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C126" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D126" t="s" s="0">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="B127" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C127" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D127" t="s" s="0">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128" t="s" s="0">
+        <v>250</v>
+      </c>
+      <c r="B128" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C128" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D128" t="s" s="0">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129" t="s" s="0">
+        <v>252</v>
+      </c>
+      <c r="B129" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C129" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D129" t="s" s="0">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A130" t="s" s="0">
+        <v>254</v>
+      </c>
+      <c r="B130" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C130" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D130" t="s" s="0">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A131" t="s" s="0">
+        <v>256</v>
+      </c>
+      <c r="B131" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C131" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D131" t="s" s="0">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A132" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="B132" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C132" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D132" t="s" s="0">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A133" t="s" s="0">
+        <v>260</v>
+      </c>
+      <c r="B133" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C133" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D133" t="s" s="0">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A134" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="B134" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C134" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D134" t="s" s="0">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A135" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="B135" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C135" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D135" t="s" s="0">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A136" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="B136" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C136" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D136" t="s" s="0">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A137" t="s" s="0">
+        <v>268</v>
+      </c>
+      <c r="B137" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C137" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D137" t="s" s="0">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A138" t="s" s="0">
+        <v>270</v>
+      </c>
+      <c r="B138" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C138" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D138" t="s" s="0">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A139" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="B139" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C139" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D139" t="s" s="0">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A140" t="s" s="0">
+        <v>274</v>
+      </c>
+      <c r="B140" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C140" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D140" t="s" s="0">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A141" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="B141" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="C141" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D141" t="s" s="0">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A142" t="s" s="0">
+        <v>276</v>
+      </c>
+      <c r="B142" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C142" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D142" t="s" s="0">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A143" t="s" s="0">
+        <v>278</v>
+      </c>
+      <c r="B143" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C143" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D143" t="s" s="0">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A144" t="s" s="0">
+        <v>280</v>
+      </c>
+      <c r="B144" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="C144" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D144" t="s" s="0">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2854,15 +3506,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="66.26953125"/>
+    <col min="1" max="1" customWidth="true" width="66.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B1" s="0" t="n">
-        <v>118.0</v>
+      <c r="B1" s="0">
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2878,7 +3530,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="0">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2886,7 +3538,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="0">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2902,7 +3554,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2957,24 +3609,24 @@
       <c r="A13" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>62.0</v>
+      <c r="B13" s="0">
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>30.0</v>
+      <c r="B14" s="0">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>32.0</v>
+      <c r="B15" s="0">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -3030,7 +3682,7 @@
         <v>108</v>
       </c>
       <c r="B22" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3043,15 +3695,15 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="35.54296875"/>
-    <col min="2" max="2" customWidth="true" width="19.26953125"/>
+    <col min="2" max="2" customWidth="true" width="19.1796875"/>
     <col min="3" max="3" customWidth="true" width="17.453125"/>
-    <col min="5" max="5" customWidth="true" width="38.7265625"/>
+    <col min="5" max="5" customWidth="true" width="38.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -3090,36 +3742,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>3</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>1</v>
+        <v>224</v>
       </c>
       <c r="D3" s="0">
-        <v>2700</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>2</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>4</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>6</v>
+        <v>224</v>
       </c>
       <c r="D4" s="0">
-        <v>5400</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>7</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new quiz feature
</commit_message>
<xml_diff>
--- a/src/main/java/data/QuizTestAppData.xlsx
+++ b/src/main/java/data/QuizTestAppData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\btl oop\quiz-test-app\src\main\java\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source\Java\OOP\quiz-test-app\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4840A02C-1321-443D-9825-342F98DCAFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE125997-DE8E-4BCB-A1E0-3F81C9B71FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5415" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionBank" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="278">
   <si>
     <t>10-6-2023 12-00-00</t>
   </si>
@@ -1154,38 +1154,6 @@
 C. Máy quét 3D</t>
   </si>
   <si>
-    <t>Phần mềm nào được sử dụng để duyệt và tìm kiếm thông tin trên Internet?</t>
-  </si>
-  <si>
-    <t>A. Google Chrome
-B. Microsoft Word
-C. Adobe Photoshop</t>
-  </si>
-  <si>
-    <t>Loại ứng dụng nào được sử dụng để giao tiếp và chia sẻ thông tin trong mạng xã hội?</t>
-  </si>
-  <si>
-    <t>A. Facebook
-B. Microsoft Excel
-C. Adobe Illustrator</t>
-  </si>
-  <si>
-    <t>ques for fun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. sbsbs
-B. snsksks
-null
-null
-null
-null
-null
-null
-null
-null
-</t>
-  </si>
-  <si>
     <t>A. sbsbs
 B. snsksks</t>
   </si>
@@ -1197,7 +1165,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1509,1990 +1476,1952 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142:L151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s" s="0">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s" s="0">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s" s="0">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="0">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s" s="0">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s" s="0">
+      <c r="D12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s" s="0">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s" s="0">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s" s="0">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s" s="0">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="0">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s" s="0">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s" s="0">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s" s="0">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s" s="0">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s" s="0">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" t="s" s="0">
+      <c r="D17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s" s="0">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>60</v>
       </c>
-      <c r="B18" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s" s="0">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s" s="0">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s" s="0">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s" s="0">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>65</v>
       </c>
-      <c r="B20" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s" s="0">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s" s="0">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>67</v>
       </c>
-      <c r="B21" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D21" t="s" s="0">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s" s="0">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>69</v>
       </c>
-      <c r="B22" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s" s="0">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s" s="0">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s" s="0">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="D23" t="s" s="0">
+      <c r="D23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s" s="0">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>73</v>
       </c>
-      <c r="B24" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s" s="0">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s" s="0">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>74</v>
       </c>
-      <c r="B25" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s" s="0">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="D25" t="s" s="0">
+      <c r="D25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s" s="0">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>75</v>
       </c>
-      <c r="B26" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C26" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D26" t="s" s="0">
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s" s="0">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s" s="0">
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s" s="0">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>78</v>
       </c>
-      <c r="B28" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s" s="0">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s" s="0">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>80</v>
       </c>
-      <c r="B29" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s" s="0">
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s" s="0">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C30" t="s" s="0">
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
         <v>37</v>
       </c>
-      <c r="D30" t="s" s="0">
+      <c r="D30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s" s="0">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>83</v>
       </c>
-      <c r="B31" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C31" t="s" s="0">
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
         <v>37</v>
       </c>
-      <c r="D31" t="s" s="0">
+      <c r="D31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s" s="0">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>84</v>
       </c>
-      <c r="B32" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C32" t="s" s="0">
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
         <v>37</v>
       </c>
-      <c r="D32" t="s" s="0">
+      <c r="D32" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s" s="0">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="B33" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C33" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s" s="0">
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s" s="0">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>86</v>
       </c>
-      <c r="B34" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C34" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D34" t="s" s="0">
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s" s="0">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>87</v>
       </c>
-      <c r="B35" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C35" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D35" t="s" s="0">
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s" s="0">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>89</v>
       </c>
-      <c r="B36" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C36" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D36" t="s" s="0">
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s" s="0">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>91</v>
       </c>
-      <c r="B37" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C37" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D37" t="s" s="0">
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s" s="0">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>92</v>
       </c>
-      <c r="B38" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C38" t="s" s="0">
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
         <v>42</v>
       </c>
-      <c r="D38" t="s" s="0">
+      <c r="D38" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s" s="0">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>94</v>
       </c>
-      <c r="B39" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C39" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D39" t="s" s="0">
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s" s="0">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>96</v>
       </c>
-      <c r="B40" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C40" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D40" t="s" s="0">
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s" s="0">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>98</v>
       </c>
-      <c r="B41" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C41" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D41" t="s" s="0">
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s" s="0">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B42" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C42" t="s" s="0">
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s">
         <v>42</v>
       </c>
-      <c r="D42" t="s" s="0">
+      <c r="D42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s" s="0">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>100</v>
       </c>
-      <c r="B43" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C43" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D43" t="s" s="0">
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s" s="0">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>102</v>
       </c>
-      <c r="B44" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C44" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D44" t="s" s="0">
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s" s="0">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>103</v>
       </c>
-      <c r="B45" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C45" t="s" s="0">
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
         <v>42</v>
       </c>
-      <c r="D45" t="s" s="0">
+      <c r="D45" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s" s="0">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>105</v>
       </c>
-      <c r="B46" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C46" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D46" t="s" s="0">
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s" s="0">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>106</v>
       </c>
-      <c r="B47" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C47" t="s" s="0">
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
         <v>42</v>
       </c>
-      <c r="D47" t="s" s="0">
+      <c r="D47" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s" s="0">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>80</v>
       </c>
-      <c r="B48" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C48" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D48" t="s" s="0">
+      <c r="B48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s" s="0">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>78</v>
       </c>
-      <c r="B49" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C49" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D49" t="s" s="0">
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s" s="0">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>81</v>
       </c>
-      <c r="B50" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C50" t="s" s="0">
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" t="s">
         <v>37</v>
       </c>
-      <c r="D50" t="s" s="0">
+      <c r="D50" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s" s="0">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>77</v>
       </c>
-      <c r="B51" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C51" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D51" t="s" s="0">
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s" s="0">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>49</v>
       </c>
-      <c r="B52" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C52" t="s" s="0">
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" t="s">
         <v>37</v>
       </c>
-      <c r="D52" t="s" s="0">
+      <c r="D52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" t="s" s="0">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>51</v>
       </c>
-      <c r="B53" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C53" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D53" t="s" s="0">
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" t="s" s="0">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>86</v>
       </c>
-      <c r="B54" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C54" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D54" t="s" s="0">
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" t="s" s="0">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>87</v>
       </c>
-      <c r="B55" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C55" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D55" t="s" s="0">
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s" s="0">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>109</v>
       </c>
-      <c r="B56" t="s" s="0">
+      <c r="B56" t="s">
         <v>19</v>
       </c>
-      <c r="C56" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D56" t="s" s="0">
+      <c r="C56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s" s="0">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>112</v>
       </c>
-      <c r="B57" t="s" s="0">
+      <c r="B57" t="s">
         <v>108</v>
       </c>
-      <c r="C57" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D57" t="s" s="0">
+      <c r="C57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s" s="0">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>114</v>
       </c>
-      <c r="B58" t="s" s="0">
+      <c r="B58" t="s">
         <v>19</v>
       </c>
-      <c r="C58" t="s" s="0">
+      <c r="C58" t="s">
         <v>42</v>
       </c>
-      <c r="D58" t="s" s="0">
+      <c r="D58" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" t="s" s="0">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>116</v>
       </c>
-      <c r="B59" t="s" s="0">
+      <c r="B59" t="s">
         <v>19</v>
       </c>
-      <c r="C59" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D59" t="s" s="0">
+      <c r="C59" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" t="s" s="0">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>118</v>
       </c>
-      <c r="B60" t="s" s="0">
+      <c r="B60" t="s">
         <v>19</v>
       </c>
-      <c r="C60" t="s" s="0">
+      <c r="C60" t="s">
         <v>37</v>
       </c>
-      <c r="D60" t="s" s="0">
+      <c r="D60" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" t="s" s="0">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>120</v>
       </c>
-      <c r="B61" t="s" s="0">
+      <c r="B61" t="s">
         <v>19</v>
       </c>
-      <c r="C61" t="s" s="0">
+      <c r="C61" t="s">
         <v>37</v>
       </c>
-      <c r="D61" t="s" s="0">
+      <c r="D61" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" t="s" s="0">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>122</v>
       </c>
-      <c r="B62" t="s" s="0">
+      <c r="B62" t="s">
         <v>19</v>
       </c>
-      <c r="C62" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D62" t="s" s="0">
+      <c r="C62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s" s="0">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>124</v>
       </c>
-      <c r="B63" t="s" s="0">
+      <c r="B63" t="s">
         <v>19</v>
       </c>
-      <c r="C63" t="s" s="0">
+      <c r="C63" t="s">
         <v>37</v>
       </c>
-      <c r="D63" t="s" s="0">
+      <c r="D63" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" t="s" s="0">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>126</v>
       </c>
-      <c r="B64" t="s" s="0">
+      <c r="B64" t="s">
         <v>19</v>
       </c>
-      <c r="C64" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D64" t="s" s="0">
+      <c r="C64" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" t="s" s="0">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>128</v>
       </c>
-      <c r="B65" t="s" s="0">
+      <c r="B65" t="s">
         <v>19</v>
       </c>
-      <c r="C65" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D65" t="s" s="0">
+      <c r="C65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s" s="0">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>130</v>
       </c>
-      <c r="B66" t="s" s="0">
+      <c r="B66" t="s">
         <v>19</v>
       </c>
-      <c r="C66" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D66" t="s" s="0">
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" t="s" s="0">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>132</v>
       </c>
-      <c r="B67" t="s" s="0">
+      <c r="B67" t="s">
         <v>19</v>
       </c>
-      <c r="C67" t="s" s="0">
+      <c r="C67" t="s">
         <v>37</v>
       </c>
-      <c r="D67" t="s" s="0">
+      <c r="D67" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" t="s" s="0">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>134</v>
       </c>
-      <c r="B68" t="s" s="0">
+      <c r="B68" t="s">
         <v>19</v>
       </c>
-      <c r="C68" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D68" t="s" s="0">
+      <c r="C68" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" t="s" s="0">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>136</v>
       </c>
-      <c r="B69" t="s" s="0">
+      <c r="B69" t="s">
         <v>19</v>
       </c>
-      <c r="C69" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D69" t="s" s="0">
+      <c r="C69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D69" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" t="s" s="0">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>138</v>
       </c>
-      <c r="B70" t="s" s="0">
+      <c r="B70" t="s">
         <v>19</v>
       </c>
-      <c r="C70" t="s" s="0">
+      <c r="C70" t="s">
         <v>42</v>
       </c>
-      <c r="D70" t="s" s="0">
+      <c r="D70" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" t="s" s="0">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>140</v>
       </c>
-      <c r="B71" t="s" s="0">
+      <c r="B71" t="s">
         <v>19</v>
       </c>
-      <c r="C71" t="s" s="0">
+      <c r="C71" t="s">
         <v>42</v>
       </c>
-      <c r="D71" t="s" s="0">
+      <c r="D71" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" t="s" s="0">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>142</v>
       </c>
-      <c r="B72" t="s" s="0">
+      <c r="B72" t="s">
         <v>19</v>
       </c>
-      <c r="C72" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D72" t="s" s="0">
+      <c r="C72" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" t="s" s="0">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>144</v>
       </c>
-      <c r="B73" t="s" s="0">
+      <c r="B73" t="s">
         <v>19</v>
       </c>
-      <c r="C73" t="s" s="0">
+      <c r="C73" t="s">
         <v>37</v>
       </c>
-      <c r="D73" t="s" s="0">
+      <c r="D73" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" t="s" s="0">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>146</v>
       </c>
-      <c r="B74" t="s" s="0">
+      <c r="B74" t="s">
         <v>19</v>
       </c>
-      <c r="C74" t="s" s="0">
+      <c r="C74" t="s">
         <v>37</v>
       </c>
-      <c r="D74" t="s" s="0">
+      <c r="D74" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" t="s" s="0">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>148</v>
       </c>
-      <c r="B75" t="s" s="0">
+      <c r="B75" t="s">
         <v>19</v>
       </c>
-      <c r="C75" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D75" t="s" s="0">
+      <c r="C75" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" t="s" s="0">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>149</v>
       </c>
-      <c r="B76" t="s" s="0">
+      <c r="B76" t="s">
         <v>19</v>
       </c>
-      <c r="C76" t="s" s="0">
+      <c r="C76" t="s">
         <v>42</v>
       </c>
-      <c r="D76" t="s" s="0">
+      <c r="D76" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" t="s" s="0">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>151</v>
       </c>
-      <c r="B77" t="s" s="0">
+      <c r="B77" t="s">
         <v>19</v>
       </c>
-      <c r="C77" t="s" s="0">
+      <c r="C77" t="s">
         <v>37</v>
       </c>
-      <c r="D77" t="s" s="0">
+      <c r="D77" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" t="s" s="0">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>153</v>
       </c>
-      <c r="B78" t="s" s="0">
+      <c r="B78" t="s">
         <v>19</v>
       </c>
-      <c r="C78" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D78" t="s" s="0">
+      <c r="C78" t="s">
+        <v>32</v>
+      </c>
+      <c r="D78" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" t="s" s="0">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>155</v>
       </c>
-      <c r="B79" t="s" s="0">
+      <c r="B79" t="s">
         <v>19</v>
       </c>
-      <c r="C79" t="s" s="0">
+      <c r="C79" t="s">
         <v>37</v>
       </c>
-      <c r="D79" t="s" s="0">
+      <c r="D79" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" t="s" s="0">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>157</v>
       </c>
-      <c r="B80" t="s" s="0">
+      <c r="B80" t="s">
         <v>19</v>
       </c>
-      <c r="C80" t="s" s="0">
+      <c r="C80" t="s">
         <v>37</v>
       </c>
-      <c r="D80" t="s" s="0">
+      <c r="D80" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" t="s" s="0">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>159</v>
       </c>
-      <c r="B81" t="s" s="0">
+      <c r="B81" t="s">
         <v>19</v>
       </c>
-      <c r="C81" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D81" t="s" s="0">
+      <c r="C81" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" t="s" s="0">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>160</v>
       </c>
-      <c r="B82" t="s" s="0">
+      <c r="B82" t="s">
         <v>19</v>
       </c>
-      <c r="C82" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D82" t="s" s="0">
+      <c r="C82" t="s">
+        <v>29</v>
+      </c>
+      <c r="D82" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A86" t="s" s="0">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>162</v>
       </c>
-      <c r="B86" t="s" s="0">
+      <c r="B86" t="s">
         <v>20</v>
       </c>
-      <c r="C86" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D86" t="s" s="0">
+      <c r="C86" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" t="s" s="0">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>164</v>
       </c>
-      <c r="B87" t="s" s="0">
+      <c r="B87" t="s">
         <v>20</v>
       </c>
-      <c r="C87" t="s" s="0">
+      <c r="C87" t="s">
         <v>42</v>
       </c>
-      <c r="D87" t="s" s="0">
+      <c r="D87" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" t="s" s="0">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>166</v>
       </c>
-      <c r="B88" t="s" s="0">
+      <c r="B88" t="s">
         <v>20</v>
       </c>
-      <c r="C88" t="s" s="0">
+      <c r="C88" t="s">
         <v>42</v>
       </c>
-      <c r="D88" t="s" s="0">
+      <c r="D88" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" t="s" s="0">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>168</v>
       </c>
-      <c r="B89" t="s" s="0">
+      <c r="B89" t="s">
         <v>20</v>
       </c>
-      <c r="C89" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D89" t="s" s="0">
+      <c r="C89" t="s">
+        <v>32</v>
+      </c>
+      <c r="D89" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A90" t="s" s="0">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>170</v>
       </c>
-      <c r="B90" t="s" s="0">
+      <c r="B90" t="s">
         <v>20</v>
       </c>
-      <c r="C90" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D90" t="s" s="0">
+      <c r="C90" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" t="s" s="0">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>172</v>
       </c>
-      <c r="B91" t="s" s="0">
+      <c r="B91" t="s">
         <v>20</v>
       </c>
-      <c r="C91" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D91" t="s" s="0">
+      <c r="C91" t="s">
+        <v>29</v>
+      </c>
+      <c r="D91" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" t="s" s="0">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>174</v>
       </c>
-      <c r="B92" t="s" s="0">
+      <c r="B92" t="s">
         <v>20</v>
       </c>
-      <c r="C92" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D92" t="s" s="0">
+      <c r="C92" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" t="s" s="0">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>176</v>
       </c>
-      <c r="B93" t="s" s="0">
+      <c r="B93" t="s">
         <v>20</v>
       </c>
-      <c r="C93" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D93" t="s" s="0">
+      <c r="C93" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A94" t="s" s="0">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>178</v>
       </c>
-      <c r="B94" t="s" s="0">
+      <c r="B94" t="s">
         <v>20</v>
       </c>
-      <c r="C94" t="s" s="0">
+      <c r="C94" t="s">
         <v>42</v>
       </c>
-      <c r="D94" t="s" s="0">
+      <c r="D94" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" t="s" s="0">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>180</v>
       </c>
-      <c r="B95" t="s" s="0">
+      <c r="B95" t="s">
         <v>20</v>
       </c>
-      <c r="C95" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D95" t="s" s="0">
+      <c r="C95" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" t="s" s="0">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>182</v>
       </c>
-      <c r="B96" t="s" s="0">
+      <c r="B96" t="s">
         <v>20</v>
       </c>
-      <c r="C96" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D96" t="s" s="0">
+      <c r="C96" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" t="s" s="0">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>184</v>
       </c>
-      <c r="B97" t="s" s="0">
+      <c r="B97" t="s">
         <v>20</v>
       </c>
-      <c r="C97" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D97" t="s" s="0">
+      <c r="C97" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" t="s" s="0">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>186</v>
       </c>
-      <c r="B98" t="s" s="0">
+      <c r="B98" t="s">
         <v>20</v>
       </c>
-      <c r="C98" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D98" t="s" s="0">
+      <c r="C98" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" t="s" s="0">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>188</v>
       </c>
-      <c r="B99" t="s" s="0">
+      <c r="B99" t="s">
         <v>20</v>
       </c>
-      <c r="C99" t="s" s="0">
+      <c r="C99" t="s">
         <v>42</v>
       </c>
-      <c r="D99" t="s" s="0">
+      <c r="D99" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" t="s" s="0">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>190</v>
       </c>
-      <c r="B100" t="s" s="0">
+      <c r="B100" t="s">
         <v>20</v>
       </c>
-      <c r="C100" t="s" s="0">
+      <c r="C100" t="s">
         <v>42</v>
       </c>
-      <c r="D100" t="s" s="0">
+      <c r="D100" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" t="s" s="0">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>192</v>
       </c>
-      <c r="B101" t="s" s="0">
+      <c r="B101" t="s">
         <v>20</v>
       </c>
-      <c r="C101" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D101" t="s" s="0">
+      <c r="C101" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" t="s" s="0">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>194</v>
       </c>
-      <c r="B102" t="s" s="0">
+      <c r="B102" t="s">
         <v>20</v>
       </c>
-      <c r="C102" t="s" s="0">
+      <c r="C102" t="s">
         <v>42</v>
       </c>
-      <c r="D102" t="s" s="0">
+      <c r="D102" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A103" t="s" s="0">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>196</v>
       </c>
-      <c r="B103" t="s" s="0">
+      <c r="B103" t="s">
         <v>20</v>
       </c>
-      <c r="C103" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D103" t="s" s="0">
+      <c r="C103" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A104" t="s" s="0">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>198</v>
       </c>
-      <c r="B104" t="s" s="0">
+      <c r="B104" t="s">
         <v>20</v>
       </c>
-      <c r="C104" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D104" t="s" s="0">
+      <c r="C104" t="s">
+        <v>29</v>
+      </c>
+      <c r="D104" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A105" t="s" s="0">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>200</v>
       </c>
-      <c r="B105" t="s" s="0">
+      <c r="B105" t="s">
         <v>20</v>
       </c>
-      <c r="C105" t="s" s="0">
+      <c r="C105" t="s">
         <v>42</v>
       </c>
-      <c r="D105" t="s" s="0">
+      <c r="D105" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" t="s" s="0">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>202</v>
       </c>
-      <c r="B106" t="s" s="0">
+      <c r="B106" t="s">
         <v>20</v>
       </c>
-      <c r="C106" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D106" t="s" s="0">
+      <c r="C106" t="s">
+        <v>29</v>
+      </c>
+      <c r="D106" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" t="s" s="0">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>204</v>
       </c>
-      <c r="B107" t="s" s="0">
+      <c r="B107" t="s">
         <v>20</v>
       </c>
-      <c r="C107" t="s" s="0">
+      <c r="C107" t="s">
         <v>42</v>
       </c>
-      <c r="D107" t="s" s="0">
+      <c r="D107" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A108" t="s" s="0">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>206</v>
       </c>
-      <c r="B108" t="s" s="0">
+      <c r="B108" t="s">
         <v>20</v>
       </c>
-      <c r="C108" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D108" t="s" s="0">
+      <c r="C108" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A109" t="s" s="0">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>208</v>
       </c>
-      <c r="B109" t="s" s="0">
+      <c r="B109" t="s">
         <v>20</v>
       </c>
-      <c r="C109" t="s" s="0">
+      <c r="C109" t="s">
         <v>42</v>
       </c>
-      <c r="D109" t="s" s="0">
+      <c r="D109" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A110" t="s" s="0">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>210</v>
       </c>
-      <c r="B110" t="s" s="0">
+      <c r="B110" t="s">
         <v>20</v>
       </c>
-      <c r="C110" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D110" t="s" s="0">
+      <c r="C110" t="s">
+        <v>29</v>
+      </c>
+      <c r="D110" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A111" t="s" s="0">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>212</v>
       </c>
-      <c r="B111" t="s" s="0">
+      <c r="B111" t="s">
         <v>20</v>
       </c>
-      <c r="C111" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D111" t="s" s="0">
+      <c r="C111" t="s">
+        <v>29</v>
+      </c>
+      <c r="D111" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A112" t="s" s="0">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>214</v>
       </c>
-      <c r="B112" t="s" s="0">
+      <c r="B112" t="s">
         <v>20</v>
       </c>
-      <c r="C112" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D112" t="s" s="0">
+      <c r="C112" t="s">
+        <v>32</v>
+      </c>
+      <c r="D112" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A113" t="s" s="0">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>216</v>
       </c>
-      <c r="B113" t="s" s="0">
+      <c r="B113" t="s">
         <v>20</v>
       </c>
-      <c r="C113" t="s" s="0">
+      <c r="C113" t="s">
         <v>42</v>
       </c>
-      <c r="D113" t="s" s="0">
+      <c r="D113" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A114" t="s" s="0">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>218</v>
       </c>
-      <c r="B114" t="s" s="0">
+      <c r="B114" t="s">
         <v>20</v>
       </c>
-      <c r="C114" t="s" s="0">
+      <c r="C114" t="s">
         <v>42</v>
       </c>
-      <c r="D114" t="s" s="0">
+      <c r="D114" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A115" t="s" s="0">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>220</v>
       </c>
-      <c r="B115" t="s" s="0">
+      <c r="B115" t="s">
         <v>20</v>
       </c>
-      <c r="C115" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D115" t="s" s="0">
+      <c r="C115" t="s">
+        <v>29</v>
+      </c>
+      <c r="D115" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A116" t="s" s="0">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>226</v>
       </c>
-      <c r="B116" t="s" s="0">
+      <c r="B116" t="s">
         <v>12</v>
       </c>
-      <c r="C116" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D116" t="s" s="0">
+      <c r="C116" t="s">
+        <v>29</v>
+      </c>
+      <c r="D116" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A117" t="s" s="0">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>228</v>
       </c>
-      <c r="B117" t="s" s="0">
+      <c r="B117" t="s">
         <v>12</v>
       </c>
-      <c r="C117" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D117" t="s" s="0">
+      <c r="C117" t="s">
+        <v>29</v>
+      </c>
+      <c r="D117" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A118" t="s" s="0">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>230</v>
       </c>
-      <c r="B118" t="s" s="0">
+      <c r="B118" t="s">
         <v>12</v>
       </c>
-      <c r="C118" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D118" t="s" s="0">
+      <c r="C118" t="s">
+        <v>32</v>
+      </c>
+      <c r="D118" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A119" t="s" s="0">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>232</v>
       </c>
-      <c r="B119" t="s" s="0">
+      <c r="B119" t="s">
         <v>12</v>
       </c>
-      <c r="C119" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D119" t="s" s="0">
+      <c r="C119" t="s">
+        <v>32</v>
+      </c>
+      <c r="D119" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A120" t="s" s="0">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>234</v>
       </c>
-      <c r="B120" t="s" s="0">
+      <c r="B120" t="s">
         <v>12</v>
       </c>
-      <c r="C120" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D120" t="s" s="0">
+      <c r="C120" t="s">
+        <v>29</v>
+      </c>
+      <c r="D120" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A121" t="s" s="0">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>236</v>
       </c>
-      <c r="B121" t="s" s="0">
+      <c r="B121" t="s">
         <v>12</v>
       </c>
-      <c r="C121" t="s" s="0">
+      <c r="C121" t="s">
         <v>42</v>
       </c>
-      <c r="D121" t="s" s="0">
+      <c r="D121" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A122" t="s" s="0">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>238</v>
       </c>
-      <c r="B122" t="s" s="0">
+      <c r="B122" t="s">
         <v>12</v>
       </c>
-      <c r="C122" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D122" t="s" s="0">
+      <c r="C122" t="s">
+        <v>29</v>
+      </c>
+      <c r="D122" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A123" t="s" s="0">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>240</v>
       </c>
-      <c r="B123" t="s" s="0">
+      <c r="B123" t="s">
         <v>12</v>
       </c>
-      <c r="C123" t="s" s="0">
+      <c r="C123" t="s">
         <v>42</v>
       </c>
-      <c r="D123" t="s" s="0">
+      <c r="D123" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A124" t="s" s="0">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>242</v>
       </c>
-      <c r="B124" t="s" s="0">
+      <c r="B124" t="s">
         <v>12</v>
       </c>
-      <c r="C124" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D124" t="s" s="0">
+      <c r="C124" t="s">
+        <v>29</v>
+      </c>
+      <c r="D124" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A125" t="s" s="0">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>244</v>
       </c>
-      <c r="B125" t="s" s="0">
+      <c r="B125" t="s">
         <v>12</v>
       </c>
-      <c r="C125" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D125" t="s" s="0">
+      <c r="C125" t="s">
+        <v>32</v>
+      </c>
+      <c r="D125" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A126" t="s" s="0">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>246</v>
       </c>
-      <c r="B126" t="s" s="0">
+      <c r="B126" t="s">
         <v>12</v>
       </c>
-      <c r="C126" t="s" s="0">
+      <c r="C126" t="s">
         <v>42</v>
       </c>
-      <c r="D126" t="s" s="0">
+      <c r="D126" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A127" t="s" s="0">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>248</v>
       </c>
-      <c r="B127" t="s" s="0">
+      <c r="B127" t="s">
         <v>12</v>
       </c>
-      <c r="C127" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D127" t="s" s="0">
+      <c r="C127" t="s">
+        <v>29</v>
+      </c>
+      <c r="D127" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A128" t="s" s="0">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>250</v>
       </c>
-      <c r="B128" t="s" s="0">
+      <c r="B128" t="s">
         <v>12</v>
       </c>
-      <c r="C128" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D128" t="s" s="0">
+      <c r="C128" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A129" t="s" s="0">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>252</v>
       </c>
-      <c r="B129" t="s" s="0">
+      <c r="B129" t="s">
         <v>12</v>
       </c>
-      <c r="C129" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D129" t="s" s="0">
+      <c r="C129" t="s">
+        <v>29</v>
+      </c>
+      <c r="D129" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A130" t="s" s="0">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>254</v>
       </c>
-      <c r="B130" t="s" s="0">
+      <c r="B130" t="s">
         <v>12</v>
       </c>
-      <c r="C130" t="s" s="0">
+      <c r="C130" t="s">
         <v>42</v>
       </c>
-      <c r="D130" t="s" s="0">
+      <c r="D130" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A131" t="s" s="0">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>256</v>
       </c>
-      <c r="B131" t="s" s="0">
+      <c r="B131" t="s">
         <v>12</v>
       </c>
-      <c r="C131" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D131" t="s" s="0">
+      <c r="C131" t="s">
+        <v>29</v>
+      </c>
+      <c r="D131" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A132" t="s" s="0">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>258</v>
       </c>
-      <c r="B132" t="s" s="0">
+      <c r="B132" t="s">
         <v>12</v>
       </c>
-      <c r="C132" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D132" t="s" s="0">
+      <c r="C132" t="s">
+        <v>32</v>
+      </c>
+      <c r="D132" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A133" t="s" s="0">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>260</v>
       </c>
-      <c r="B133" t="s" s="0">
+      <c r="B133" t="s">
         <v>12</v>
       </c>
-      <c r="C133" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D133" t="s" s="0">
+      <c r="C133" t="s">
+        <v>32</v>
+      </c>
+      <c r="D133" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A134" t="s" s="0">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>262</v>
       </c>
-      <c r="B134" t="s" s="0">
+      <c r="B134" t="s">
         <v>12</v>
       </c>
-      <c r="C134" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D134" t="s" s="0">
+      <c r="C134" t="s">
+        <v>29</v>
+      </c>
+      <c r="D134" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A135" t="s" s="0">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>264</v>
       </c>
-      <c r="B135" t="s" s="0">
+      <c r="B135" t="s">
         <v>12</v>
       </c>
-      <c r="C135" t="s" s="0">
+      <c r="C135" t="s">
         <v>42</v>
       </c>
-      <c r="D135" t="s" s="0">
+      <c r="D135" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A136" t="s" s="0">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>266</v>
       </c>
-      <c r="B136" t="s" s="0">
+      <c r="B136" t="s">
         <v>12</v>
       </c>
-      <c r="C136" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D136" t="s" s="0">
+      <c r="C136" t="s">
+        <v>32</v>
+      </c>
+      <c r="D136" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A137" t="s" s="0">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>268</v>
       </c>
-      <c r="B137" t="s" s="0">
+      <c r="B137" t="s">
         <v>12</v>
       </c>
-      <c r="C137" t="s" s="0">
+      <c r="C137" t="s">
         <v>42</v>
       </c>
-      <c r="D137" t="s" s="0">
+      <c r="D137" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A138" t="s" s="0">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>270</v>
       </c>
-      <c r="B138" t="s" s="0">
+      <c r="B138" t="s">
         <v>12</v>
       </c>
-      <c r="C138" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D138" t="s" s="0">
+      <c r="C138" t="s">
+        <v>29</v>
+      </c>
+      <c r="D138" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A139" t="s" s="0">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>272</v>
       </c>
-      <c r="B139" t="s" s="0">
+      <c r="B139" t="s">
         <v>12</v>
       </c>
-      <c r="C139" t="s" s="0">
+      <c r="C139" t="s">
         <v>42</v>
       </c>
-      <c r="D139" t="s" s="0">
+      <c r="D139" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A140" t="s" s="0">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>274</v>
       </c>
-      <c r="B140" t="s" s="0">
+      <c r="B140" t="s">
         <v>12</v>
       </c>
-      <c r="C140" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D140" t="s" s="0">
+      <c r="C140" t="s">
+        <v>29</v>
+      </c>
+      <c r="D140" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A141" t="s" s="0">
-        <v>283</v>
-      </c>
-      <c r="B141" t="s" s="0">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>277</v>
+      </c>
+      <c r="B141" t="s">
         <v>108</v>
       </c>
-      <c r="C141" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D141" t="s" s="0">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A142" t="s" s="0">
+      <c r="C141" t="s">
+        <v>29</v>
+      </c>
+      <c r="D141" t="s">
         <v>276</v>
-      </c>
-      <c r="B142" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C142" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D142" t="s" s="0">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A143" t="s" s="0">
-        <v>278</v>
-      </c>
-      <c r="B143" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C143" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D143" t="s" s="0">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A144" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B144" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="C144" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D144" t="s" s="0">
-        <v>281</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3504,184 +3433,184 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="66.1796875"/>
+    <col min="1" max="1" width="66.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="0">
+      <c r="B1">
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s" s="0">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s" s="0">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s" s="0">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s" s="0">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s" s="0">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s" s="0">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s" s="0">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s" s="0">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s" s="0">
+      <c r="B15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="B17" s="0">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s" s="0">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s" s="0">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s" s="0">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s" s="0">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s" s="0">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="0">
+      <c r="B22">
         <v>2</v>
       </c>
     </row>
@@ -3698,79 +3627,79 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.54296875"/>
-    <col min="2" max="2" customWidth="true" width="19.1796875"/>
-    <col min="3" max="3" customWidth="true" width="17.453125"/>
-    <col min="5" max="5" customWidth="true" width="38.81640625"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0">
+      <c r="D1">
         <v>2700</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>5400</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>222</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>223</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>224</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>30</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>222</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>223</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>224</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>30</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update function GUI 6
</commit_message>
<xml_diff>
--- a/src/main/java/data/QuizTestAppData.xlsx
+++ b/src/main/java/data/QuizTestAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\btl oop\quiz-test-app\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4840A02C-1321-443D-9825-342F98DCAFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A2BA7F-02EC-45BF-8ACF-257E75D0C7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionBank" sheetId="1" r:id="rId1"/>
@@ -38,31 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="284">
-  <si>
-    <t>10-6-2023 12-00-00</t>
-  </si>
-  <si>
-    <t>10-7-2023 12-00-00</t>
-  </si>
-  <si>
-    <t>1,3,5,7,8,9,11,12,13,14,16,18,20,22,24,30</t>
-  </si>
-  <si>
-    <t>Kiem tra giua ki 1 cong nghe</t>
-  </si>
-  <si>
-    <t>Kiem tra giua ki 1 toan</t>
-  </si>
-  <si>
-    <t>12-6-2023 12-00-00</t>
-  </si>
-  <si>
-    <t>10-8-2023 12-00-00</t>
-  </si>
-  <si>
-    <t>1,4,5,7,8,9,10,12,13,14,16,18,20,22,24,30</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="311">
   <si>
     <t>root</t>
   </si>
@@ -473,22 +449,6 @@
     <t>root/Default</t>
   </si>
   <si>
-    <t>Đây là câu hỏi thi giữa kỳ sinh học 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. Yes
-B. No
-null
-null
-null
-null
-null
-null
-null
-null
-</t>
-  </si>
-  <si>
     <t>Quá trình tiêu hóa thức ăn diễn ra chủ yếu ở đâu trong cơ thể người?</t>
   </si>
   <si>
@@ -552,9 +512,6 @@
 D. Rễ</t>
   </si>
   <si>
-    <t>12. Chất nào sau đây là chất chủ yếu tạo nên tế bào trong cơ thể chúng ta?</t>
-  </si>
-  <si>
     <t>A. Carbohydrate
 B. Chất béo
 C. Protein
@@ -588,18 +545,12 @@
 D. Insulin</t>
   </si>
   <si>
-    <t>16. Quá trình nào sau đây giúp cây sản xuất thức ăn?</t>
-  </si>
-  <si>
     <t>A. Quang hợp
 B. Hô hấp
 C. Tiêu hóa
 D. Tuần hoàn</t>
   </si>
   <si>
-    <t>17. Chất gì trong máu chịu trách nhiệm vận chuyển oxy đến các tế bào trong cơ thể?</t>
-  </si>
-  <si>
     <t>A. Glucose
 B. Hemoglobin
 C. Insulin
@@ -645,9 +596,6 @@
     <t>22. Quá trình nào sau đây giúp cây tiếp nhận carbon dioxide từ không khí?</t>
   </si>
   <si>
-    <t>23. Chất gì trong miễn dịch giúp phát hiện và tiêu diệt vi khuẩn và virus?</t>
-  </si>
-  <si>
     <t>A. Antigen
 B. Antibody
 C. Hormone
@@ -942,18 +890,6 @@
 C. Canada</t>
   </si>
   <si>
-    <t>Thi gi do</t>
-  </si>
-  <si>
-    <t>10/9/2023</t>
-  </si>
-  <si>
-    <t>11/9/2023</t>
-  </si>
-  <si>
-    <t>1, 4, 7, 9</t>
-  </si>
-  <si>
     <t>Đơn vị đo dung lượng bộ nhớ được sử dụng trong máy tính là:</t>
   </si>
   <si>
@@ -986,14 +922,6 @@
 C. Ổ cứng di động</t>
   </si>
   <si>
-    <t>Giao thức truyền thông phổ biến trong mạng Internet là:</t>
-  </si>
-  <si>
-    <t>A. HTTP
-B. FTP
-C. SMTP</t>
-  </si>
-  <si>
     <t>Đâu không phải là phần cứng của máy tính?</t>
   </si>
   <si>
@@ -1066,14 +994,6 @@
 C. Ethernet</t>
   </si>
   <si>
-    <t>Loại kết nối dùng để truyền âm thanh và hình ảnh chất lượng cao từ máy tính ra TV là:</t>
-  </si>
-  <si>
-    <t>A. VGA
-B. HDMI
-C. DVI</t>
-  </si>
-  <si>
     <t>Phần mềm nào được sử dụng để tạo bài thuyết trình?</t>
   </si>
   <si>
@@ -1130,28 +1050,12 @@
 C. HDMI</t>
   </si>
   <si>
-    <t>Phần mềm nào được sử dụng để xử lý và tính toán dữ liệu số lớn?</t>
-  </si>
-  <si>
-    <t>A. Microsoft Excel
-B. Adobe Photoshop
-C. Google Chrome</t>
-  </si>
-  <si>
     <t>Công nghệ nào cho phép truyền tải dữ liệu không dây trong phạm vi gần?</t>
   </si>
   <si>
     <t>A. Wi-Fi
 B. NFC
 C. Ethernet</t>
-  </si>
-  <si>
-    <t>Loại máy quét nào được sử dụng để chuyển đổi tài liệu giấy thành dạng số?</t>
-  </si>
-  <si>
-    <t>A. Máy quét phẳng
-B. Máy quét mã vạch
-C. Máy quét 3D</t>
   </si>
   <si>
     <t>Phần mềm nào được sử dụng để duyệt và tìm kiếm thông tin trên Internet?</t>
@@ -1191,6 +1095,183 @@
   </si>
   <si>
     <t>ques for fun abcdefxyz</t>
+  </si>
+  <si>
+    <t>root/Default/Linh tinh</t>
+  </si>
+  <si>
+    <t>What is the correct answer to this question? Dòng cuối cùng là dòng ANSWER, mô tả đáp án đúng. Sau từ ANSWER là một dấu hai chấm và một khoảng trắng, tiếp đến là một ký tự viết hoa sau cho ký tự này nằm trong danh sách các đáp án ở trên. Sau dòng ANSWER phải có một dòng trống</t>
+  </si>
+  <si>
+    <t>A. Is it this one?
+B. Maybe this answer?
+C. Possibly this one?
+D. Must be this one!</t>
+  </si>
+  <si>
+    <t>Which LMS has the most quiz import formats?</t>
+  </si>
+  <si>
+    <t>A. Moodle
+B. ATutor
+C. Claroline
+D. Blackboard
+E. WebCT</t>
+  </si>
+  <si>
+    <t>Why did the chicken cross the road?</t>
+  </si>
+  <si>
+    <t>A. To get to the other side
+B. It wanted to live dangerously
+C. It saw Frank Perdue coming
+D. No one knows
+E. No one cares
+F. sjsjjsjs
+G. hshshssuus</t>
+  </si>
+  <si>
+    <t>Huy is very handsome, is’nt he?</t>
+  </si>
+  <si>
+    <t>A. Yes, he is
+B. Ofcourse
+C. No, I don’t think so</t>
+  </si>
+  <si>
+    <t>We will get A+ OOP, alright?</t>
+  </si>
+  <si>
+    <t>A. Ofcourse, we are
+B. No, it is terrible, we get A</t>
+  </si>
+  <si>
+    <t>Trường bị gay, đm nó</t>
+  </si>
+  <si>
+    <t>A. Ừ
+B. Không, nó thẳng như cây đũa vậy</t>
+  </si>
+  <si>
+    <t>Loại computer nào được sử dụng phổ biến trong việc xử lý đồ họa và video?</t>
+  </si>
+  <si>
+    <t>Loại nào được sử dụng để giao tiếp và chia sẻ thông tin trong mạng xã hội?</t>
+  </si>
+  <si>
+    <t>23. Chất nào trong miễn dịch giúp phát hiện và tiêu diệt vi khuẩn và virus?</t>
+  </si>
+  <si>
+    <t>Quá trình nào sau đây giúp cây sản xuất thức ăn?</t>
+  </si>
+  <si>
+    <t>Chất gì trong máu chịu trách nhiệm vận chuyển oxy đến các tế bào trong cơ thể?</t>
+  </si>
+  <si>
+    <t>Đây là một câu hỏi thi giữa kỳ sinh học 7</t>
+  </si>
+  <si>
+    <t>A. Yes
+B. No</t>
+  </si>
+  <si>
+    <t>Chất nào sau đây là chất chủ yếu tạo nên tế bào trong cơ thể chúng ta?</t>
+  </si>
+  <si>
+    <t>Kiểm tra cuối kỳ hệ điều hành</t>
+  </si>
+  <si>
+    <t>21/June/2023</t>
+  </si>
+  <si>
+    <t>22/June/2023</t>
+  </si>
+  <si>
+    <t>Thi giữa kỳ môn công nghệ lớp 7</t>
+  </si>
+  <si>
+    <t>21/March/2023</t>
+  </si>
+  <si>
+    <t>Baka</t>
+  </si>
+  <si>
+    <t>1,3,5,7,9,11,18,102,20,26</t>
+  </si>
+  <si>
+    <t>null,140</t>
+  </si>
+  <si>
+    <t>null,140,142</t>
+  </si>
+  <si>
+    <t>null,140,142,144</t>
+  </si>
+  <si>
+    <t>null,140,142,144,145</t>
+  </si>
+  <si>
+    <t>1,3,5,7,9,11,18,102,20,26,0</t>
+  </si>
+  <si>
+    <t>1,3,5,7,9,11,18,102,20,26,0,2</t>
+  </si>
+  <si>
+    <t>1,3,5,7,9,11,18,102,20,26,0,2,4</t>
+  </si>
+  <si>
+    <t>1,3,5,7,9,11,18,102,20,26,0,2,4,6</t>
+  </si>
+  <si>
+    <t>1,3,5,7,9,11,18,102,20,26,0,2,4,6,54</t>
+  </si>
+  <si>
+    <t>Thi cuối kỳ sinh học 7</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>,56</t>
+  </si>
+  <si>
+    <t>,56,57</t>
+  </si>
+  <si>
+    <t>,56,57,58</t>
+  </si>
+  <si>
+    <t>,142,144,145</t>
+  </si>
+  <si>
+    <t>,140,144,145</t>
+  </si>
+  <si>
+    <t>,140,145</t>
+  </si>
+  <si>
+    <t>,140</t>
+  </si>
+  <si>
+    <t>,140,145,142</t>
+  </si>
+  <si>
+    <t>,140,145,142,143</t>
+  </si>
+  <si>
+    <t>,140,145,142,143,141</t>
+  </si>
+  <si>
+    <t>,140,145,142,143,141,112</t>
+  </si>
+  <si>
+    <t>,1,3,5,7,9,11,18,102,20,0,2,4,6,54</t>
+  </si>
+  <si>
+    <t>,1,3,5,7,9,11,18,102,20,0,4,6,54</t>
+  </si>
+  <si>
+    <t>,1,5,7,9,11,18,102,20,0,4,6,54</t>
   </si>
 </sst>
 </file>
@@ -1509,1986 +1590,2056 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C27" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C29" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s" s="0">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C37" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D37" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s" s="0">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s" s="0">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C48" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D48" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s" s="0">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D51" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C51" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D51" t="s" s="0">
-        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s" s="0">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s" s="0">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s" s="0">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s" s="0">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s" s="0">
-        <v>112</v>
+        <v>276</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>108</v>
+        <v>11</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>113</v>
+        <v>277</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s" s="0">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s" s="0">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>128</v>
+        <v>278</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s" s="0">
-        <v>136</v>
+        <v>274</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s" s="0">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s" s="0">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s" s="0">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s" s="0">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s" s="0">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D74" t="s" s="0">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s" s="0">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s" s="0">
-        <v>149</v>
+        <v>273</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D76" t="s" s="0">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s" s="0">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D77" t="s" s="0">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s" s="0">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s" s="0">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D79" t="s" s="0">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s" s="0">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D80" t="s" s="0">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s" s="0">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D81" t="s" s="0">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s" s="0">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D82" t="s" s="0">
-        <v>161</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C83" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D83" t="s" s="0">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="B84" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C84" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D84" t="s" s="0">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="B85" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C85" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D85" t="s" s="0">
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s" s="0">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B86" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D86" t="s" s="0">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s" s="0">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D87" t="s" s="0">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s" s="0">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D88" t="s" s="0">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s" s="0">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D89" t="s" s="0">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s" s="0">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D90" t="s" s="0">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s" s="0">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D91" t="s" s="0">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s" s="0">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D92" t="s" s="0">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s" s="0">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D93" t="s" s="0">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s" s="0">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D94" t="s" s="0">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s" s="0">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D95" t="s" s="0">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s" s="0">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D96" t="s" s="0">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s" s="0">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s" s="0">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C98" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s" s="0">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C99" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s" s="0">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B100" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s" s="0">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B101" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D101" t="s" s="0">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s" s="0">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B102" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C102" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D102" t="s" s="0">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s" s="0">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B103" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D103" t="s" s="0">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s" s="0">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D104" t="s" s="0">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s" s="0">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B105" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D105" t="s" s="0">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s" s="0">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C106" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D106" t="s" s="0">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s" s="0">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C107" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D107" t="s" s="0">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s" s="0">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B108" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C108" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D108" t="s" s="0">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s" s="0">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B109" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D109" t="s" s="0">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s" s="0">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B110" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C110" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D110" t="s" s="0">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s" s="0">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D111" t="s" s="0">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s" s="0">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B112" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C112" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D112" t="s" s="0">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s" s="0">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B113" t="s" s="0">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C113" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D113" t="s" s="0">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s" s="0">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s" s="0">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C114" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D114" t="s" s="0">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s" s="0">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B115" t="s" s="0">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C115" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D115" t="s" s="0">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s" s="0">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B116" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C116" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D116" t="s" s="0">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s" s="0">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B117" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C117" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D117" t="s" s="0">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s" s="0">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B118" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D118" t="s" s="0">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s" s="0">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B119" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D119" t="s" s="0">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s" s="0">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B120" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C120" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D120" t="s" s="0">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s" s="0">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B121" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D121" t="s" s="0">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s" s="0">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B122" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C122" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D122" t="s" s="0">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s" s="0">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B123" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D123" t="s" s="0">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s" s="0">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B124" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C124" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D124" t="s" s="0">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s" s="0">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B125" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C125" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D125" t="s" s="0">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s" s="0">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B126" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C126" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D126" t="s" s="0">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s" s="0">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="B127" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C127" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D127" t="s" s="0">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s" s="0">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B128" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C128" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D128" t="s" s="0">
-        <v>251</v>
+        <v>235</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s" s="0">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B129" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C129" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D129" t="s" s="0">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s" s="0">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B130" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C130" t="s" s="0">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D130" t="s" s="0">
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s" s="0">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B131" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C131" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D131" t="s" s="0">
-        <v>257</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s" s="0">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="B132" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C132" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D132" t="s" s="0">
-        <v>259</v>
+        <v>243</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s" s="0">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="B133" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C133" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D133" t="s" s="0">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s" s="0">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="B134" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C134" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D134" t="s" s="0">
-        <v>263</v>
+        <v>247</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s" s="0">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="B135" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C135" t="s" s="0">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D135" t="s" s="0">
-        <v>265</v>
+        <v>249</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s" s="0">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B136" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C136" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D136" t="s" s="0">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s" s="0">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B137" t="s" s="0">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C137" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D137" t="s" s="0">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s" s="0">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D138" t="s" s="0">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s" s="0">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="B139" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s" s="0">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D139" t="s" s="0">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s" s="0">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="B140" t="s" s="0">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C140" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D140" t="s" s="0">
-        <v>275</v>
+        <v>255</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s" s="0">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="B141" t="s" s="0">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="C141" t="s" s="0">
         <v>29</v>
       </c>
       <c r="D141" t="s" s="0">
-        <v>282</v>
+        <v>260</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s" s="0">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="B142" t="s" s="0">
-        <v>12</v>
+        <v>258</v>
       </c>
       <c r="C142" t="s" s="0">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D142" t="s" s="0">
-        <v>277</v>
+        <v>262</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s" s="0">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="B143" t="s" s="0">
-        <v>12</v>
+        <v>258</v>
       </c>
       <c r="C143" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D143" t="s" s="0">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s" s="0">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="B144" t="s" s="0">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="C144" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D144" t="s" s="0">
-        <v>281</v>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A145" t="s" s="0">
+        <v>267</v>
+      </c>
+      <c r="B145" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="C145" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D145" t="s" s="0">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A146" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="B146" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="C146" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D146" t="s" s="0">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3498,10 +3649,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7375D0D9-A088-4E33-84C0-F60360358F66}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3511,23 +3662,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B2" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0">
         <v>86</v>
@@ -3535,7 +3686,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0">
         <v>86</v>
@@ -3543,7 +3694,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0">
         <v>0</v>
@@ -3551,7 +3702,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0">
         <v>30</v>
@@ -3559,7 +3710,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0">
         <v>0</v>
@@ -3567,7 +3718,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0">
         <v>0</v>
@@ -3575,7 +3726,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B9" s="0">
         <v>0</v>
@@ -3583,7 +3734,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B10" s="0">
         <v>0</v>
@@ -3591,7 +3742,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B11" s="0">
         <v>0</v>
@@ -3599,7 +3750,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0">
         <v>0</v>
@@ -3607,7 +3758,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0">
         <v>63</v>
@@ -3615,7 +3766,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B14" s="0">
         <v>31</v>
@@ -3623,7 +3774,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B15" s="0">
         <v>32</v>
@@ -3631,7 +3782,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B16" s="0">
         <v>0</v>
@@ -3639,7 +3790,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0">
         <v>56</v>
@@ -3647,7 +3798,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0">
         <v>0</v>
@@ -3655,7 +3806,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0">
         <v>0</v>
@@ -3663,7 +3814,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0">
         <v>0</v>
@@ -3671,7 +3822,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0">
         <v>0</v>
@@ -3679,10 +3830,18 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B22" s="0">
         <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s" s="0">
+        <v>258</v>
+      </c>
+      <c r="B23" s="0">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3694,8 +3853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E57CE46-9D74-4C06-8F20-8319158C49B7}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3708,70 +3867,67 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>3</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>1</v>
+        <v>281</v>
       </c>
       <c r="D1" s="0">
-        <v>2700</v>
+        <v>5400</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>2</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>4</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>5</v>
+        <v>283</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>283</v>
       </c>
       <c r="D2" s="0">
-        <v>5400</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>7</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>222</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>223</v>
+        <v>283</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>224</v>
+        <v>283</v>
       </c>
       <c r="D3" s="0">
-        <v>30</v>
+        <v>600</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s" s="0">
-        <v>222</v>
+        <v>295</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>223</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>224</v>
-      </c>
-      <c r="D4" s="0">
-        <v>30</v>
+        <v>283</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>7200.0</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>225</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add gif image feature
</commit_message>
<xml_diff>
--- a/src/main/java/data/QuizTestAppData.xlsx
+++ b/src/main/java/data/QuizTestAppData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source\Java\OOP\quiz-test-app\src\main\java\data\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="285">
   <si>
     <t>10-6-2023 12-00-00</t>
   </si>
@@ -1192,11 +1192,20 @@
   <si>
     <t>ques for fun abcdefxyz</t>
   </si>
+  <si>
+    <t xml:space="preserve">N
+N
+N
+N
+G
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1508,7 +1517,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -1516,1981 +1525,1984 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="50.28515625"/>
+    <col min="2" max="2" customWidth="true" width="42.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s" s="0">
         <v>52</v>
       </c>
+      <c r="E11" t="s" s="0">
+        <v>284</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s" s="0">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B15" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B16" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B18" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B19" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s" s="0">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B20" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s" s="0">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B21" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s" s="0">
         <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B22" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s" s="0">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="0">
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s" s="0">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B26" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s" s="0">
         <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B27" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B28" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s" s="0">
         <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B29" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" t="s" s="0">
         <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" t="s" s="0">
         <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B33" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s" s="0">
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B34" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s" s="0">
         <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="B35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="B35" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s" s="0">
         <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="B36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="B36" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s" s="0">
         <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B37" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D37" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="B38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="B39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="B39" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s" s="0">
         <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B40" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s" s="0">
         <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="B41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B41" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D41" t="s" s="0">
         <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="B43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B43" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s" s="0">
         <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="B44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="B44" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D44" t="s" s="0">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="B45" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B45" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" t="s" s="0">
         <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="B46" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s" s="0">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="B47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" t="s" s="0">
         <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="B48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="B48" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="B49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="B49" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s" s="0">
         <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="B50" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B50" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C50" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="B51" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D51" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="B52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B52" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C52" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C53" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="B53" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D53" t="s" s="0">
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="B54" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="B54" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s" s="0">
         <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="B55" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="B55" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D55" t="s" s="0">
         <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C56" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="C56" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s" s="0">
         <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="C57" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D57" t="s" s="0">
         <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C59" t="s">
-        <v>29</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C59" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D59" t="s" s="0">
         <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" t="s" s="0">
         <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" t="s" s="0">
         <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C62" t="s">
-        <v>32</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="C62" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D62" t="s" s="0">
         <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" t="s" s="0">
         <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" t="s" s="0">
         <v>126</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C64" t="s">
-        <v>29</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="C64" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D64" t="s" s="0">
         <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" t="s" s="0">
         <v>128</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C65" t="s">
-        <v>32</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="C65" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D65" t="s" s="0">
         <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C66" t="s">
-        <v>29</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="C66" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D66" t="s" s="0">
         <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" t="s" s="0">
         <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="C68" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D68" t="s" s="0">
         <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C69" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C69" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D69" t="s" s="0">
         <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" t="s" s="0">
         <v>138</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" t="s" s="0">
         <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" t="s" s="0">
         <v>140</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" t="s" s="0">
         <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" t="s" s="0">
         <v>142</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C72" t="s">
-        <v>29</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C72" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D72" t="s" s="0">
         <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" t="s" s="0">
         <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" t="s" s="0">
         <v>146</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" t="s" s="0">
         <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" t="s" s="0">
         <v>148</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C75" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="C75" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D75" t="s" s="0">
         <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" t="s" s="0">
         <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" t="s" s="0">
         <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C78" t="s">
-        <v>32</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C78" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D78" t="s" s="0">
         <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" t="s" s="0">
         <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" t="s" s="0">
         <v>157</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" t="s" s="0">
         <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C81" t="s">
-        <v>29</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="C81" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D81" t="s" s="0">
         <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C82" t="s">
-        <v>29</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="C82" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D82" t="s" s="0">
         <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" t="s" s="0">
         <v>162</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C86" t="s">
-        <v>29</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C86" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D86" t="s" s="0">
         <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" t="s" s="0">
         <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" t="s" s="0">
         <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C89" t="s">
-        <v>32</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C89" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D89" t="s" s="0">
         <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C90" t="s">
-        <v>29</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="C90" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D90" t="s" s="0">
         <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" t="s" s="0">
         <v>172</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C91" t="s">
-        <v>29</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="C91" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D91" t="s" s="0">
         <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C92" t="s">
-        <v>29</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="C92" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D92" t="s" s="0">
         <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C93" t="s">
-        <v>29</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="C93" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D93" t="s" s="0">
         <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" t="s" s="0">
         <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C95" t="s">
-        <v>29</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="C95" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D95" t="s" s="0">
         <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C96" t="s">
-        <v>32</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="C96" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D96" t="s" s="0">
         <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C97" t="s">
-        <v>32</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C97" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D97" t="s" s="0">
         <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C98" t="s">
-        <v>29</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C98" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D98" t="s" s="0">
         <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" t="s" s="0">
         <v>188</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" t="s" s="0">
         <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" t="s" s="0">
         <v>190</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" t="s" s="0">
         <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C101" t="s">
-        <v>29</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="C101" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D101" t="s" s="0">
         <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" t="s" s="0">
         <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C103" t="s">
-        <v>29</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="C103" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D103" t="s" s="0">
         <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C104" t="s">
-        <v>29</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="C104" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D104" t="s" s="0">
         <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" t="s" s="0">
         <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C106" t="s">
-        <v>29</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="C106" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D106" t="s" s="0">
         <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" t="s" s="0">
         <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C108" t="s">
-        <v>32</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="C108" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D108" t="s" s="0">
         <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" t="s" s="0">
         <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" t="s" s="0">
         <v>210</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C110" t="s">
-        <v>29</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="C110" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D110" t="s" s="0">
         <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C111" t="s">
-        <v>29</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C111" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D111" t="s" s="0">
         <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C112" t="s">
-        <v>32</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="C112" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D112" t="s" s="0">
         <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" t="s" s="0">
         <v>216</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" t="s" s="0">
         <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" t="s" s="0">
         <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C115" t="s">
-        <v>29</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="C115" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D115" t="s" s="0">
         <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C116" t="s">
-        <v>29</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="C116" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D116" t="s" s="0">
         <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C117" t="s">
-        <v>29</v>
-      </c>
-      <c r="D117" t="s">
+      <c r="C117" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D117" t="s" s="0">
         <v>229</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" t="s" s="0">
         <v>230</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C118" t="s">
-        <v>32</v>
-      </c>
-      <c r="D118" t="s">
+      <c r="C118" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D118" t="s" s="0">
         <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" t="s" s="0">
         <v>232</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C119" t="s">
-        <v>32</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="C119" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D119" t="s" s="0">
         <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" t="s" s="0">
         <v>234</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C120" t="s">
-        <v>29</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="C120" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D120" t="s" s="0">
         <v>235</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" t="s" s="0">
         <v>236</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" t="s" s="0">
         <v>237</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" t="s" s="0">
         <v>238</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C122" t="s">
-        <v>29</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="C122" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D122" t="s" s="0">
         <v>239</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" t="s" s="0">
         <v>240</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" t="s" s="0">
         <v>241</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="A124" t="s" s="0">
         <v>242</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C124" t="s">
-        <v>29</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="C124" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D124" t="s" s="0">
         <v>243</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" t="s" s="0">
         <v>244</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C125" t="s">
-        <v>32</v>
-      </c>
-      <c r="D125" t="s">
+      <c r="C125" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D125" t="s" s="0">
         <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" t="s" s="0">
         <v>246</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" t="s" s="0">
         <v>247</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" t="s" s="0">
         <v>248</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C127" t="s">
-        <v>29</v>
-      </c>
-      <c r="D127" t="s">
+      <c r="C127" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D127" t="s" s="0">
         <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="A128" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C128" t="s">
-        <v>29</v>
-      </c>
-      <c r="D128" t="s">
+      <c r="C128" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D128" t="s" s="0">
         <v>251</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" t="s" s="0">
         <v>252</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C129" t="s">
-        <v>29</v>
-      </c>
-      <c r="D129" t="s">
+      <c r="C129" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D129" t="s" s="0">
         <v>253</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" t="s" s="0">
         <v>254</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" t="s" s="0">
         <v>255</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" t="s" s="0">
         <v>256</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C131" t="s">
-        <v>29</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="C131" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D131" t="s" s="0">
         <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" t="s" s="0">
         <v>258</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C132" t="s">
-        <v>32</v>
-      </c>
-      <c r="D132" t="s">
+      <c r="C132" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D132" t="s" s="0">
         <v>259</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" t="s" s="0">
         <v>260</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C133" t="s">
-        <v>32</v>
-      </c>
-      <c r="D133" t="s">
+      <c r="C133" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D133" t="s" s="0">
         <v>261</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" t="s" s="0">
         <v>262</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C134" t="s">
-        <v>29</v>
-      </c>
-      <c r="D134" t="s">
+      <c r="C134" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D134" t="s" s="0">
         <v>263</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" t="s" s="0">
         <v>264</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" t="s" s="0">
         <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" t="s" s="0">
         <v>266</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C136" t="s">
-        <v>32</v>
-      </c>
-      <c r="D136" t="s">
+      <c r="C136" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D136" t="s" s="0">
         <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" t="s" s="0">
         <v>268</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" t="s" s="0">
         <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" t="s" s="0">
         <v>270</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C138" t="s">
-        <v>29</v>
-      </c>
-      <c r="D138" t="s">
+      <c r="C138" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D138" t="s" s="0">
         <v>271</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" t="s" s="0">
         <v>272</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" t="s" s="0">
         <v>273</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" t="s" s="0">
         <v>274</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C140" t="s">
-        <v>29</v>
-      </c>
-      <c r="D140" t="s">
+      <c r="C140" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D140" t="s" s="0">
         <v>275</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" t="s" s="0">
         <v>283</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C141" t="s">
-        <v>29</v>
-      </c>
-      <c r="D141" t="s">
+      <c r="C141" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D141" t="s" s="0">
         <v>282</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" t="s" s="0">
         <v>276</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C142" t="s">
-        <v>29</v>
-      </c>
-      <c r="D142" t="s">
+      <c r="C142" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D142" t="s" s="0">
         <v>277</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="A143" t="s" s="0">
         <v>278</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C143" t="s">
-        <v>29</v>
-      </c>
-      <c r="D143" t="s">
+      <c r="C143" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D143" t="s" s="0">
         <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="A144" t="s" s="0">
         <v>280</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="C144" t="s">
-        <v>29</v>
-      </c>
-      <c r="D144" t="s">
+      <c r="C144" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D144" t="s" s="0">
         <v>281</v>
       </c>
     </row>
@@ -3509,182 +3521,182 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="66.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="0">
         <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="0">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="0">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
+      <c r="A17" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B17" s="0">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="0">
         <v>2</v>
       </c>
     </row>
@@ -3703,77 +3715,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.5703125"/>
+    <col min="2" max="2" customWidth="true" width="19.140625"/>
+    <col min="3" max="3" customWidth="true" width="17.42578125"/>
+    <col min="5" max="5" customWidth="true" width="38.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="0">
         <v>2700</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>5400</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update image and gif
</commit_message>
<xml_diff>
--- a/src/main/java/data/QuizTestAppData.xlsx
+++ b/src/main/java/data/QuizTestAppData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\btl oop\quiz-test-app\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6122E3DE-7F7A-4783-896C-CBA7F9939EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04FC818-044B-4E63-9797-E092553491B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="456">
   <si>
     <t>10-6-2023 12-00-00</t>
   </si>
@@ -47,18 +47,6 @@
   </si>
   <si>
     <t>Kiem tra giua ki 1 cong nghe</t>
-  </si>
-  <si>
-    <t>Kiem tra giua ki 1 toan</t>
-  </si>
-  <si>
-    <t>12-6-2023 12-00-00</t>
-  </si>
-  <si>
-    <t>10-8-2023 12-00-00</t>
-  </si>
-  <si>
-    <t>1,4,5,7,8,9,10,12,13,14,16,18,20,22,24,30</t>
   </si>
   <si>
     <t>root</t>
@@ -1216,7 +1204,8 @@
     <t>,2,22,21,25,23,7,15,19,9,13,20,17,3,5,6,10,8,14,4,12,16,11,0,18</t>
   </si>
   <si>
-    <t xml:space="preserve">P
+    <t xml:space="preserve">N
+P
 P
 P
 P
@@ -1225,11 +1214,10 @@
 N
 N
 N
-N
 </t>
   </si>
   <si>
-    <t xml:space="preserve">N
+    <t xml:space="preserve">P
 N
 N
 N
@@ -1240,6 +1228,745 @@
 N
 N
 </t>
+  </si>
+  <si>
+    <t>Quiz có ảnh</t>
+  </si>
+  <si>
+    <t>QUIZ sinh học</t>
+  </si>
+  <si>
+    <t>,65,81,61,63,60,62,55,64,80</t>
+  </si>
+  <si>
+    <t>What's name of this planet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G
+N
+N
+N
+N
+N
+N
+N
+N
+N
+</t>
+  </si>
+  <si>
+    <t>,141,142,143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. Earth
+B. Sun
+C. Satturn
+</t>
+  </si>
+  <si>
+    <t>Bạn biết bao nhiêu hệ điều hành?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. 1
+B. 2
+C. 3
+</t>
+  </si>
+  <si>
+    <t>root/Bảo hiểm</t>
+  </si>
+  <si>
+    <t>Đối với sản phẩm bảo hiểm liên kết đơn vị, phí chuyển đổi quỹ liên kết đơn vị là:</t>
+  </si>
+  <si>
+    <t>A. Khoản phí dùng để trang trải chi phí phát hành hợp đồng bảo hiểm, chi phí thẩm định bảo hiểm, chi phí kiểm tra y tế, chi hoa hồng đại lý và chi phí khác.
+B. Khoản phí bên mua bảo hiểm phải trả cho doanh nghiệp bảo hiểm khi thực hiện chuyển đổi tài sản đầu tư giữa các quỹ liên kết đơn vị.
+C. Khoản phí để bù đắp chi phí liên quan đến việc duy trì hợp đồng bảo hiểm và cung cấp thông tin liên quan đến hợp đồng bảo hiểm cho bên mua bảo hiểm.
+D. Khoản phí đối với quyền lợi bảo hiểm rủi ro theo cam kết tại hợp đồng bảo hiểm.</t>
+  </si>
+  <si>
+    <t>2. Theo quy định của Pháp luật, Văn phòng đại diện của doanh nghiệp bảo hiểm, doanh nghiệp môi giới bảo hiểm nước ngoài tại Việt Nam được thực hiện hoạt động nào sau đây:</t>
+  </si>
+  <si>
+    <t>A. Xúc tiến xây dựng các dự án đầu tư của doanh nghiệp bảo hiểm, doanh nghiệp môi giới bảo hiểm nước ngoài.
+B. Thúc đẩy và theo dõi việc thực hiện các dự án do doanh nghiệp bảo hiểm, doanh nghiệp môi giới bảo hiểm nước ngoài tài trợ tại Việt Nam.
+C. Nghiên cứu thị trường.
+D. A, B, C đúng.</t>
+  </si>
+  <si>
+    <t>3. Đại lý bảo hiểm không có quyền nào sau đây:</t>
+  </si>
+  <si>
+    <t>A. Yêu cầu doanh nghiệp bảo hiểm hoàn trả tiền ký quĩ hoặc thế chấp tài sản theo thỏa thuận trong hợp đồng đại lý bảo hiểm.
+B. Tham dự các lớp đào tạo, bồi dưỡng, nâng cao trình độ cho đại lý bảo hiểm do doanh nghiệp bảo hiểm tổ chức.
+C. Ký thay khách hàng.
+D. Hưởng hoa hồng và các quyền, lợi ích hợp pháp khác từ hoạt động đại lý bảo hiểm.</t>
+  </si>
+  <si>
+    <t>4. Anh A 33 tuổi tham gia một hợp đồng Bảo Hiểm Ung Thư 360 vào ngày 01/05/2019 với STBH 01 tỷ đồng. Trong thời gian hợp đồng có hiệu lực, anh A lần lượt gặp các rủi ro sau: Ngày 04/07/2025: được chẩn đoán mắc ung thư dạ dày giai đoạn sớm.  Ngày 30/10/2025: phẫu thuật tái tạo hình dạng dạ dày (Phẫu Thuật Phục Hồi). Ngày 07/09/2028: tử vong do tai nạn. Giả sử các sự kiện trên đều được Manulife chấp thuận chi trả, tổng số tiền mà anh A sẽ nhận được là: </t>
+  </si>
+  <si>
+    <t>A. 1,7 tỷ đồng. 
+B. 2,7 tỷ đồng. 
+C. 1,5 tỷ đồng. 
+D. 2,5 tỷ đồng.</t>
+  </si>
+  <si>
+    <t>5. Khách hàng A tham gia Sản phẩm Bảo hiểm Ung Thư 360 vào ngày 1/1/2019 với số tiền bảo hiểm là 500 triệu đồng. Ngày 17/03/2019, khách hàng A được chẩn đoán mắc ung thư giai đoạn sớm. Quyền lợi ung thư giai đoạn sớm khách hàng A nhận được là:</t>
+  </si>
+  <si>
+    <t>A. 250 triệu đồng
+B. 300 triệu đồng
+C. 0 đồng
+D. 500 triệu đồng</t>
+  </si>
+  <si>
+    <t>6. Kể từ sau thời điểm Manulife đồng ý chi trả quyền lợi Ung Thư Giai Đoạn Cuối cho Người Được Bảo Hiểm của hợp đồng Bảo hiểm Ung Thư 360, vào mỗi ngày kỷ niệm hợp đồng hàng tháng, Manulife sẽ chi trả QLBH Trợ Cấp Thu Nhập bằng:</t>
+  </si>
+  <si>
+    <t>A. 1% Số Tiền Bảo Hiểm
+B. 0,5% Số Tiền Bảo Hiểm
+C. 1,5% Số Tiền Bảo Hiểm</t>
+  </si>
+  <si>
+    <t>7. Doanh nghiệp bảo hiểm có quyền từ chối trả tiền bảo hiểm cho người thụ hưởng hoặc từ chối bồi thường cho người được bảo hiểm trong trường hợp:</t>
+  </si>
+  <si>
+    <t>A. Sự kiện bảo hiểm xảy ra không thuộc phạm vi trách nhiệm bảo hiểm theo thỏa thuận trong hợp đồng bảo hiểm (A).
+B. Sự kiện bảo hiểm xảy ra thuộc các trường hợp loại trừ trách nhiệm bảo hiểm theo thỏa thuận trong hợp đồng bảo hiểm (B).
+C. Sự kiện bảo hiểm xảy ra trong thời gian gia hạn nộp phí bảo hiểm.  
+D. A, B đúng. </t>
+  </si>
+  <si>
+    <t>8. Đối với hợp đồng bảo hiểm con người, trường hợp một hoặc một số người thụ hưởng cố ý gây ra cái chết hoặc thương tật vĩnh viễn cho người được bảo hiểm thì:</t>
+  </si>
+  <si>
+    <t>A. Doanh nghiệp bảo hiểm không phải trả tiền bảo hiểm.
+B. Doanh nghiệp bảo hiểm vẫn trả tiền cho tất cả người thụ hưởng bảo hiểm.
+C. Doanh nghiệp bảo hiểm vẫn phải trả tiền bảo hiểm cho những người thụ hưởng khác theo thoả thuận trong hợp đồng bảo hiểm.
+D. Không trường hợp nào đúng.</t>
+  </si>
+  <si>
+    <t>9. Doanh nghiệp bảo hiểm có nghĩa vụ:</t>
+  </si>
+  <si>
+    <t>A. Chi trả tất cả các chi phí khai thác hợp đồng bảo hiểm cho đại lý ngoài hoa hồng bảo hiểm (A).
+B. Yêu cầu đại lý bảo hiểm phải có tài sản thế chấp.
+C. Chịu trách nhiệm về những thiệt hại hay tổn thất do hoạt động đại lý bảo hiểm của mình gây ra theo thỏa thuận trong hợp đồng đại lý bảo hiểm (C).
+D. A, C đúng.</t>
+  </si>
+  <si>
+    <t>10. Trong Sản phẩm Bảo hiểm Ung Thư 360, quyền lợi nào sau đây sẽ chấm dứt ngay khi Manulife chấp nhận chi trả:</t>
+  </si>
+  <si>
+    <t>A. Quyền lợi bảo hiểm Ung Thư Giai Đoạn Cuối
+B. Quyền lợi bảo hiểm Ung Thư Chi Phí Lớn
+C. Quyền lợi bảo hiểm Miễn Đóng Phí
+D. Cả ba đáp án A, B và C.</t>
+  </si>
+  <si>
+    <t>11. Khách hàng A tham gia Sản phẩm Bảo hiểm Ung Thư 360 với số tiền bảo hiểm là 800 triệu đồng. Trong thời gian hợp đồng có hiệu lực, khách hàng A được chẩn đoán mắc 2 bệnh ung thư giai đoạn sớm thuộc phạm vi bảo hiểm, được chẩn đoán trong cùng 1 ngày. Tổng quyền lợi ung thư giai đoạn sớm khách hàng nhận được là:</t>
+  </si>
+  <si>
+    <t>A. 480 triệu đồng
+B. 920 triệu đồng
+C. 600 triệu đồng
+D. 800 triệu đồng</t>
+  </si>
+  <si>
+    <t>12. Theo qui định của Pháp luật, chương trình đào tạo Phần kiến thức chung dành cho đại lý bảo hiểm gồm:</t>
+  </si>
+  <si>
+    <t>A. Kiến thức chung về bảo hiểm; Pháp luật về kinh doanh bảo hiểm
+B. Trách nhiệm của đại lý, đạo đức hành nghề đại lý; Quyền và nghĩa vụ của doanh nghiệp bảo hiểm, chi nhánh doanh nghiệp bảo hiểm phi nhân thọ nước ngoài, đại lý bảo hiểm trong hoạt động đại lý bảo hiểm
+C. Kỹ năng bán bảo hiểm
+D. Cả A,B,C</t>
+  </si>
+  <si>
+    <t>13. Mức vốn pháp định của doanh nghiệp bảo hiểm nhân thọ, kinh doanh bảo hiểm nhân thọ (trừ bảo hiểm liên kết đơn vị, bảo hiểm hưu trí) và bảo hiểm sức khỏe là:</t>
+  </si>
+  <si>
+    <t>A. 1.000 tỷ đồng Việt Nam
+B. 800 tỷ đồng Việt Nam
+C. 600 tỷ đồng Việt Nam
+D. 300 tỷ đồng Việt Nam</t>
+  </si>
+  <si>
+    <t>14. Đại lý bảo hiểm không được doanh nghiệp bảo hiểm uỷ quyền tiến hành hoạt động nào dưới đây:</t>
+  </si>
+  <si>
+    <t>A. Thu xếp việc giao kết hợp đồng bảo hiểm.
+B. Thu xếp giải quyết bồi thường, trả tiền bảo hiểm khi xảy ra sự kiện bảo hiểm.
+C. Thu phí bảo hiểm.
+D. Trực tiếp ký kết hợp đồng bảo hiểm.</t>
+  </si>
+  <si>
+    <t>15. Theo Luật kinh doanh bảo hiểm, thời gian 15 ngày là quy định về thời hạn nào trong những thời hạn dưới đây:</t>
+  </si>
+  <si>
+    <t>A. Thời hiệu khởi kiện về hợp đồng bảo hiểm, kể từ ngày pháp sinh tranh chấp.
+B. Thời hạn doanh nghiệp bảo hiểm phải trả tiền bảo hiểm hoặc bồi thường kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường (trừ trường hợp có thỏa thuận khác về thời hạn trong hợp đồng bảo hiểm).
+C. Thời hạn yêu cầu trả tiền bảo hiểm hoặc bồi thường theo hợp đồng bảo hiểm, kể từ ngày xảy ra sự kiện bảo hiểm.</t>
+  </si>
+  <si>
+    <t>16.  Chọn 1 phương án đúng về đặc điểm của nghiệp vụ bảo hiểm trọn đời:</t>
+  </si>
+  <si>
+    <t>A. Doanh nghiệp bảo hiểm trả tiền bảo hiểm cho người thụ hưởng khi bên mua bảo hiểm chết ở bất kỳ thời điểm nào trong suốt cuộc đời của người đó
+B. Doanh nghiệp bảo hiểm trả tiền bảo hiểm cho người thụ hưởng khi người được bảo hiểm vẫn sống tại thời điểm kết thúc hiệu lực hợp đồng
+C. Doanh nghiệp bảo hiểm trả tiền bảo hiểm cho người thụ hưởng khi người được bảo hiểm chết vào bất kỳ thời điểm nào trong suốt cuộc đời của người đó</t>
+  </si>
+  <si>
+    <t>17. Trong trường hợp NĐBH của Sản phẩm Bảo hiểm Ung Thư 360 tử vong và Manulife đã chi trả QLBH Trợ Cấp Thu Nhập vượt quá thời điểm này, Manulife sẽ: </t>
+  </si>
+  <si>
+    <t>A. Không cấn trừ số tiền đã chi trả dư vào quyền lợi Tử Vong. 
+B. Cấn trừ số tiền đã chi trả dư vào quyền lợi Tử Vong. 
+C. Cả hai đáp án trên đều đúng. </t>
+  </si>
+  <si>
+    <t>18. Chọn phương án sai về trường hợp Hợp đồng bảo hiểm vô hiệu:</t>
+  </si>
+  <si>
+    <t>A. Tại thời điểm giao kết hợp đồng bảo hiểm, đối tượng bảo hiểm không tồn tại.
+B. Tại thời điểm giao kết hợp đồng bảo hiểm, bên mua bảo hiểm biết sự kiện bảo hiểm đã xảy ra.
+C. Đại lý bảo hiểm không nộp phí bảo hiểm đã thu của bên mua bảo hiểm cho doanh nghiệp bảo hiểm.
+D. Bên mua bảo hiểm không có quyền lợi có thể được bảo hiểm.</t>
+  </si>
+  <si>
+    <t>19. Đại lý bảo hiểm không được tranh giành khách hàng dưới các hình thức ngăn cản, lôi kéo, mua chuộc, đe dọa nhân viên hoặc khách hàng của:</t>
+  </si>
+  <si>
+    <t>A. Doanh nghiệp bảo hiểm khác
+B. Đại lý bảo hiểm khác
+C. Doanh nghiệp môi giới bảo hiểm khác
+D. Cả A, B, C</t>
+  </si>
+  <si>
+    <t>20. Theo quy định của Pháp luật, hợp đồng bảo hiểm chấm dứt nếu bên mua bảo hiểm không đóng đủ phí bảo hiểm hoặc không đóng phí bảo hiểm theo thời hạn thỏa thuận trong hợp đồng bảo hiểm (trừ trường hợp các bên có thỏa thuận khác). Khi đó, bên mua bảo hiểm vẫn phải đóng đủ phí bảo hiểm đến thời điểm chấm dứt hợp đồng bảo hiểm nếu hợp đồng bảo hiểm đó là:</t>
+  </si>
+  <si>
+    <t>A. Hợp đồng bảo hiểm con người (A)
+B. Hợp đồng bảo hiểm tài sản (B)
+C. Hợp đồng bảo hiểm trách nhiệm dân sự (C)
+D. B, C đúng</t>
+  </si>
+  <si>
+    <t>21. Trong Sản phẩm Bảo hiểm Ung Thư 360, trong trường hợp con của Người Được Bảo Hiểm được Manulife chấp thuận cấp quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của Người Được Bảo Hiểm, ngày bắt đầu bảo hiểm sẽ là:</t>
+  </si>
+  <si>
+    <t>A. Ngày Manulife đồng ý cấp quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của Người Được Bảo Hiểm
+B. Ngày Manulife chấp nhận chi trả quyền lợi Ung Thư Giai Đoạn Cuối cho Người Được Bảo Hiểm.
+C. Ngày hoàn thành hồ sơ yêu cầu cấp quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của Người Được Bảo Hiểm
+D. Ngày Người Được Bảo Hiểm được chẩn đoán mắc bệnh Ung Thư Giai Đoạn Cuối</t>
+  </si>
+  <si>
+    <t>22. Khoản tiền mà bên mua bảo hiểm đóng cho doanh nghiệp bảo hiểm theo thỏa thuận trong hợp đồng bảo hiểm là:</t>
+  </si>
+  <si>
+    <t>A. Số tiền bảo hiểm.
+B. Giá trị bảo hiểm.
+C. Số tiền bồi thường.
+D. Phí bảo hiểm.</t>
+  </si>
+  <si>
+    <t>23. Trong trường hợp không có thỏa thuận về thời hạn, doanh nghiệp bảo hiểm phải trả tiền bảo hiểm hoặc bồi thường cho người được bảo hiểm trong vòng:</t>
+  </si>
+  <si>
+    <t>A. 45 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường.
+B. 30 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường. 
+C. 60 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường.
+D. 15 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường. </t>
+  </si>
+  <si>
+    <t>24. Việc yêu cầu tham gia bảo hiểm được thực hiện bởi: </t>
+  </si>
+  <si>
+    <t>A. Môi giới bảo hiểm.
+B. Doanh nghiệp bảo hiểm
+C. Đại lý bảo hiểm.
+D. Bên mua bảo hiểm.</t>
+  </si>
+  <si>
+    <t>25. Trong nghiệp vụ bảo hiểm trả tiền định kỳ, khi người được bảo hiểm còn sống nhưng chưa đạt đến thời hạn nhất định theo thỏa thuận trong hợp đồng bảo hiểm, doanh nghiệp bảo hiểm có trách nhiệm:</t>
+  </si>
+  <si>
+    <t>A. Chi trả tiền bảo hiểm cho Bên mua bảo hiểm
+B. Chi trả tiền bảo hiểm cho Người thụ hưởng
+C. Không chi trả bất cứ quyền lợi bảo hiểm nào cả
+D. Chi trả tiền bảo hiểm cho Người được bảo hiểm</t>
+  </si>
+  <si>
+    <t>26. Đại lý bảo hiểm có thể:</t>
+  </si>
+  <si>
+    <t>A. Lựa chọn và ký kết hợp đồng đại lý bảo hiểm đối với doanh nghiệp bảo hiểm theo đúng quy định pháp luật
+B. Yêu cầu doanh nghiệp bảo hiểm hoàn trả tiền ký quỹ hoặc tài sản thế chấp theo thỏa thuận trong hợp đồng đại lý bảo hiểm
+C. Sửa đổi, bổ sung điều khoản trong hợp đồng bảo hiểm theo ý kiến của bên mua bảo hiểm
+D. A, B đúng</t>
+  </si>
+  <si>
+    <t>27. Tỷ lệ hoa hồng tối đa tính trên phí bảo hiểm của hợp đồng bảo hiểm nhân thọ cá nhân đối với nghiệp vụ bảo hiểm trả tiền định kỳ, phương thức nộp phí bảo hiểm 1 lần là:</t>
+  </si>
+  <si>
+    <t>A. 10%
+B. 15%
+C. 5%
+D. 7%</t>
+  </si>
+  <si>
+    <t>28. Chọn một phương án đúng về các đặc điểm của sản phẩm bảo hiểm nhân thọ hỗn hợp</t>
+  </si>
+  <si>
+    <t>A. Có giá trị hoàn lại, có chia lãi hoặc không chia lãi
+B. Có cả 2 yếu tố bảo vệ và tiết kiệm
+C. A, B đúng
+D. Không có đáp án đúng</t>
+  </si>
+  <si>
+    <t>29. Chọn phương án đúng về nghiệp vụ bảo hiểm mà doanh nghiệp bảo hiểm nhân thọ và phi nhân thọ đều được triển khai:</t>
+  </si>
+  <si>
+    <t>A. Bảo hiểm hưu trí.
+B. Bảo hiểm tài sản.
+C. Bảo hiểm sức khỏe.
+D. Không trường hợp nào đúng.</t>
+  </si>
+  <si>
+    <t>30. Đại lý bảo hiểm có thể được lựa chọn và ký kết hợp đồng đại lý bảo hiểm với đối tượng nào dưới đây:</t>
+  </si>
+  <si>
+    <t>A. Doanh nghiệp bảo hiểm nhân thọ, doanh nghiệp bảo hiểm phi nhân thọ
+B. Doanh nghiệp bảo hiểm sức khỏe, doanh nghiệp tái bảo hiểm
+C. Chi nhánh doanh nghiệp bảo hiểm phi nhân thọ nước ngoài
+D. Cả A, B, C</t>
+  </si>
+  <si>
+    <t>31. Trong trường hợp bên mua bảo hiểm chứng minh được rằng họ không biết thời điểm xảy ra sự kiện bảo hiểm thì thời hạn yêu cầu trả tiền bảo hiểm hoặc bồi thường là:</t>
+  </si>
+  <si>
+    <t>A. 1 năm kể từ ngày xảy ra sự kiện bảo hiểm.
+B. 1 năm kể từ ngày bên mua bảo hiểm biết việc xảy ra sự kiện bảo hiểm.
+C.  2 năm kể từ ngày xảy ra sự kiện bảo hiểm.
+D. 2 năm kể từ ngày bên mua bảo hiểm biết việc xảy ra sự kiện bảo hiểm.</t>
+  </si>
+  <si>
+    <t>32. Bên mua bảo hiểm đã đóng phí bảo hiểm nhân thọ từ hai năm trở lên, nhưng không thể đóng các khoản phí bảo hiểm tiếp theo thì sau thời hạn 60 ngày, kể từ ngày gia hạn đóng phí, trừ trường hợp các bên có thỏa thuận khác, doanh nghiệp bảo hiểm có quyền đơn phương đình chỉ hợp đồng và bên mua bảo hiểm:</t>
+  </si>
+  <si>
+    <t>A. Nhận giá trị hoàn lại của hợp đồng bảo hiểm
+B. Không có quyền đòi lại khoản phí bảo hiểm đã đóng
+C. Nhận lại toàn bộ phí bảo hiểm đã đóng</t>
+  </si>
+  <si>
+    <t>33. Quỹ bảo vệ người được bảo hiểm được thành lập tại doanh nghiệp bảo hiểm nhằm bảo vệ quyền lợi của người được bảo hiểm trong trường hợp nào sau đây:</t>
+  </si>
+  <si>
+    <t>A. Người được bảo hiểm bị thất nghiệp 
+B. Doanh nghiệp bảo hiểm phá sản hoặc mất khả năng thanh toán
+C. Người được bảo hiểm gặp khó khăn về tài chính, không có khả năng đóng phí bảo hiểm
+D. Người được bảo hiểm gặp rủi ro do chiến tranh, động đất</t>
+  </si>
+  <si>
+    <t>34. Phát biểu nào sau đây là đúng về QLBH Ung Thư Chi Phí Lớn của Sản phẩm Bảo hiểm Ung Thư 360: </t>
+  </si>
+  <si>
+    <t>A. Chi trả 100% STBH khi NĐBH được chẩn đoán Ung Thư Giai Đoạn Sớm hoặc Ung Thư Giai Đoạn Cuối thuộc danh sách bệnh Ung Thư Chi Phí Lớn. QLBH này sẽ chấm dứt ngay sau khi Manulife chi trả quyền lợi Ung Thư Giai Đoạn Sớm hoặc Ung Thư Giai Đoạn Cuối. 
+B. Chi trả 100% STBH khi NĐBH được chẩn đoán Ung Thư Giai Đoạn Cuối thuộc danh sách bệnh Ung Thư Chi Phí Lớn. QLBH nàysẽ chấm dứt ngay sau khi Manulife chi trả QLBH Ung Thư Giai Đoạn Sớm hoặc Ung Thư Giai Đoạn Cuối. 
+C. Chi trả 50% STBH khi NĐBH được chẩn đoán Ung Thư Giai Đoạn Cuối thuộc danh sách bệnh Ung Thư Chi Phí Lớn. QLBH này sẽ chấm dứt ngay sau khi Manulife chấp nhận chi trả hoặc khi QLBH Ung Thư Giai Đoạn Cuối đã được chi trả. 
+D. Chi trả 50% STBH khi NĐBH được chẩn đoán Ung Thư Giai Đoạn Sớm hoặc Ung Thư Giai Đoạn Cuối thuộc danh sách bệnh Ung Thư Chi Phí Lớn. QLBH này sẽ chấm dứt ngay sau khi Manulife chi trả QLBH Ung Thư Giai Đoạn Sớm hoặc Ung Thư Giai Đoạn Cuối. </t>
+  </si>
+  <si>
+    <t>35. Luật kinh doanh bảo hiểm quy định Bên mua bảo hiểm đóng phí bảo hiểm nhân thọ theo cách:</t>
+  </si>
+  <si>
+    <t>A. Đóng một lần theo quy định bắt buộc của Doanh nghiệp bảo hiểm
+B. Đóng nhiều lần theo quy định bắt buộc của Doanh nghiệp bảo hiểm
+C. Đóng một lần hoặc nhiều lần theo thời hạn, phương thức thỏa thuận trong hợp đồng bảo hiểm
+D. A, B, C sai</t>
+  </si>
+  <si>
+    <t>36. Ngày 1/1/2019, khách hàng A tham gia Sản phẩm Bảo hiểm Ung Thư 360. Đến 31/5/2020, khách hàng A được chẩn đoán mắc ung thư giai đoạn cuối, thuộc danh mục ung thư chi phí lớn, các quyền lợi mà khách hàng A nhận được là:</t>
+  </si>
+  <si>
+    <t>A. 150% số tiền bảo hiểm + quyền lợi miễn đóng phí +  quyền lợi trợ cấp thu nhập + quyền lợi miễn phí dành cho con
+B. 150% số tiền bảo hiểm + quyền lợi miễn đóng phí + quyền lợi miễn phí dành cho con
+C. 105% số tiền bảo hiểm + quyền lợi miễn đóng phí + quyền lợi trợ cấp thu nhập + quyền lợi miễn phí dành cho con
+D. 160% số tiền bảo hiểm + quyền lợi miễn đóng phí + quyền lợi trợ cấp thu nhập + quyền lợi miễn phí dành cho con </t>
+  </si>
+  <si>
+    <t>37. Theo quy định của Pháp luật, phát biểu nào dưới đây sai:</t>
+  </si>
+  <si>
+    <t>A. Kinh doanh bảo hiểm là hoạt động của doanh nghiệp bảo hiểm nhằm mục đích sinh lợi, theo đó doanh nghiệp bảo hiểm nhận một khoản phí bảo hiểm của doanh nghiệp bảo hiểm khác để cam kết bồi thường cho các trách nhiệm đã nhận bảo hiểm.
+B. Hoạt động đại lý bảo hiểm là hoạt động giới thiệu, chào bán bảo hiểm, thu xếp việc giao kết hợp đồng bảo hiểm và các công việc khác nhằm thực hiện hợp đồng bảo hiểm theo ủy quyền của doanh nghiệp bảo hiểm.
+C. Sự kiện bảo hiểm là sự kiện khách quan do các bên thỏa thuận hoặc pháp luật quy định mà khi sự kiện đó xảy ra thì doanh nghiệp bảo hiểm phải trả tiền bảo hiểm cho người thụ hưởng hoặc bồi thường cho người được bảo hiểm.</t>
+  </si>
+  <si>
+    <t>38. Cơ quan có trách nhiệm kiểm tra, giám sát hoạt động đào tạo đại lý bảo hiểm là:</t>
+  </si>
+  <si>
+    <t>A. Bộ Tài chính.
+B. Bộ Công thương.
+C. Hiệp hội bảo hiểm Việt Nam.
+D. Bộ Giáo dục và Đào tạo.</t>
+  </si>
+  <si>
+    <t>39. Theo quy định của pháp luật về kinh doanh bảo hiểm, các sản phẩm thuộc nghiệp vụ bảo hiểm nhân thọ trước khi triển khai phải được:</t>
+  </si>
+  <si>
+    <t>A. Bộ Tài chính phê chuẩn quy tắc, điều khoản, biểu phí
+B. Đăng ký quy tắc, điều khoản, biểu phí với Hiệp hội Bảo hiểm Việt Nam
+C. Đăng ký quy tắc, điều khoản, biểu phí với Bộ Tài chính
+D. Hiệp hội Bảo hiểm Việt Nam phê chuẩn quy tắc, điều khoản, biểu phí</t>
+  </si>
+  <si>
+    <t>40. Ý nào dưới đây là đúng về thời hạn bảo hiểm của Quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của Người Được Bảo Hiểm trong Sản phẩm Bảo hiểm Ung Thư 360:</t>
+  </si>
+  <si>
+    <t>A. Thời hạn bảo hiểm tối đa là 20 năm
+B. Tuổi bảo hiểm tối đa là 30 tuổi
+C. Đáp án A hoặc B tùy thời điểm nào đến trước</t>
+  </si>
+  <si>
+    <t>1. Giá trị hoàn lại của một hợp đồng bảo hiểm liên kết chung được xác định:</t>
+  </si>
+  <si>
+    <t>A. Là giá trị hợp đồng đó trong quỹ liên kết chung vào ngày hủy bỏ hợp đồng bảo hiểm trừ đi phí quản lý hợp đồng bảo hiểm.
+B. Là giá trị hợp đồng đó trong quỹ liên kết chung vào ngày kết thúc hợp đồng bảo hiểm
+C. Là giá trị hợp đồng đó trong quỹ liên kết chung vào ngày hủy bỏ hợp đồng bảo hiểm
+D. Là giá trị hợp đồng đó trong quỹ liên kết chung vào ngày hủy bỏ hợp đồng bảo hiểm trừ đi phí hủy bỏ hợp đồng bảo hiểm.</t>
+  </si>
+  <si>
+    <t>2. Theo Pháp luật kinh doanh bảo hiểm, văn phòng đại diện của doanh nghiệp bảo hiểm, doanh nghiệp môi giới bảo hiểm nước ngoài tại Việt Nam không được thực hiện hoạt động nào sau đây:</t>
+  </si>
+  <si>
+    <t>A. Thúc đẩy và theo dõi việc thực hiện các dự án do doanh nghiệp bảo hiểm, doanh nghiệp môi giới bảo hiểm nước ngoài tài trợ tại Việt Nam.
+B. Kinh doanh bảo hiểm.
+C. Nghiên cứu thị trường
+D. Xúc tiến xây dựng các dự án đầu tư của doanh nghiệp bảo hiểm, doanh nghiệp môi giới bảo hiểm nước ngoài.</t>
+  </si>
+  <si>
+    <t>3. Chi quản lý đại lý của doanh nghiệp bảo hiểm, chi nhánh nước ngoài không bao gồm:</t>
+  </si>
+  <si>
+    <t>A. Chi đào tạo nâng cao kiến thức cho đại lý.
+B. Chi tuyển dụng đại lý, khen thưởng đại lý và hỗ trợ đại lý.
+C. Chi đào tạo ban đầu và thi cấp chứng chỉ đại lý.
+D. Chi hoa hồng bảo hiểm.</t>
+  </si>
+  <si>
+    <t>4. Thời hạn đóng phí và thời hạn hợp đồng của Sản phẩm Bảo hiểm Ung Thư 360 là: </t>
+  </si>
+  <si>
+    <t>A. Thời hạn đóng phí 10 năm; Thời hạn hợp đồng 10 năm 
+B. Thời hạn đóng phí 10 năm; Thời hạn hợp đồng đến khi NĐBH 99 tuổi 
+C. Thời hạn đóng phí 10 năm; Thời hạn hợp đồng 12 năm 
+D. Thời hạn đóng phí 12 năm; Thời hạn hợp đồng đến khi NĐBH 99 tuổi</t>
+  </si>
+  <si>
+    <t>5. Trong Sản phẩm Bảo hiểm Ung thư 360, trường hợp NĐBH là trẻ em 1,5 tuổi số tiền bảo hiểm chi trả khi các sự kiện bảo hiểm xảy ra được điều chỉnh theo tỷ lệ % là bao nhiêu:</t>
+  </si>
+  <si>
+    <t>A. 40%
+B. 60%
+C. 20%
+D. 80%</t>
+  </si>
+  <si>
+    <t>6. Khách hàng A của hợp đồng Sản phẩm Bảo hiểm Ung Thư 360 được chẩn đoán mắc ung thư giai đoạn cuối, quyền lợi bảo hiểm giai đoạn cuối đã được chi trả, hợp đồng của khách hàng A sẽ chấm dứt hiệu lực, đúng hay sai?</t>
+  </si>
+  <si>
+    <t>A. Đúng
+B. Sai</t>
+  </si>
+  <si>
+    <t>7. Trong trường hợp không có thỏa thuận về thời hạn, doanh nghiệp bảo hiểm phải trả tiền bảo hiểm hoặc bồi thường cho người được bảo hiểm trong vòng:</t>
+  </si>
+  <si>
+    <t>A. 60 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường.
+B. 45 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường.
+C. 30 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường. 
+D. 15 ngày kể từ ngày nhận được đầy đủ hồ sơ hợp lệ về yêu cầu trả tiền bảo hiểm hoặc bồi thường. </t>
+  </si>
+  <si>
+    <t>8. Trường hợp nào dưới đây doanh nghiệp bảo hiểm phải trả tiền bảo hiểm trong hợp đồng bảo hiểm con người:</t>
+  </si>
+  <si>
+    <t>A. Người được bảo hiểm chết do bị thi hành án tử hình
+B. Người được bảo hiểm chết hoặc bị thương tật vĩnh viễn do lỗi cố ý của bên mua bảo hiểm
+C. Người được bảo hiểm chết do tự tử trong thời hạn hai năm, kể từ ngày nộp khoản phí bảo hiểm đầu tiên hoặc kể từ ngày hợp đồng bảo hiểm tiếp tục có hiệu lực
+D. Người được bảo hiểm chết do tự tử sau thời hạn hai năm, kể từ ngày nộp khoản phí bảo hiểm đầu tiên hoặc kể từ ngày hợp đồng bảo hiểm tiếp tục có hiệu lực</t>
+  </si>
+  <si>
+    <t>9. Phát biểu nào sau đây là sai về nội dung hoạt động đại lý bảo hiểm:</t>
+  </si>
+  <si>
+    <t>A. Giới thiệu, chào bán bảo hiểm
+B. Thu phí bảo hiểm.
+C. Hỗ trợ giảm phí bảo hiểm hoặc khuyến mại khách hàng tham gia bảo hiểm.
+D. A, B đúng.</t>
+  </si>
+  <si>
+    <t>10. Phát biểu nào sau đây là đúng về quyền lợi Hỗ Trợ Trượt Giá của Sản phẩm Bảo hiểm Ung Thư 360: </t>
+  </si>
+  <si>
+    <t>A. Tương đương 5% STBH từ năm hợp đồng đầu tiên, mỗi năm sau đó cộng thêm 5% STBH (A). 
+B. Được chi trả cùng với quyền lợi Ung Thư Giai Đoạn Cuối (B). 
+C. Mỗi đầu năm hợp đồng, BMBH cần cung cấp bằng chứng NĐBH còn sống. Quyền lợi này sẽ chấm dứt sau khi Manulife đã chi trả đủ 60 lần, hoặc sau khi NĐBH tử vong. 
+D. A và B là đáp án đúng. </t>
+  </si>
+  <si>
+    <t>11. Ngày 1/1/2019, khách hàng A tham gia Sản phẩm Bảo hiểm Ung Thư 360. Đến 31/5/2020, khách hàng A được chẩn đoán mắc ung thư giai đoạn cuối, thuộc danh mục ung thư chi phí lớn. Ngày 9/6/2020, khách hàng A tử vong. Các quyền lợi mà khách hàng A nhận được là:</t>
+  </si>
+  <si>
+    <t>A. 150% số tiền bảo hiểm + quyền lợi miễn đóng phí + quyền lợi trợ cấp thu nhập + quyền lợi miễn phí dành cho con + quyền lợi tử vong
+B. 150% số tiền bảo hiểm + quyền lợi miễn đóng phí + quyền lợi miễn phí dành cho con+ quyền lợi tử vong
+C. 105% số tiền bảo hiểm + quyền lợi miễn đóng phí + quyền lợi trợ cấp thu nhập + quyền lợi miễn phí dành cho con + quyền lợi tử vong
+D. 160% số tiền bảo hiểm + quyền lợi miễn đóng phí + quyền lợi trợ cấp thu nhập + quyền lợi miễn phí dành cho con + quyền lợi tử vong</t>
+  </si>
+  <si>
+    <t>12. Đại lý bảo hiểm là:</t>
+  </si>
+  <si>
+    <t>A. Người được doanh nghiệp bảo hiểm ủy quyền thực hiện tất cả các công việc liên quan đến nghiệp vụ bảo hiểm.
+B. Tổ chức, cá nhân được doanh nghiệp bảo hiểm ủy quyền trên cơ sở hợp đồng đại lý bảo hiểm để thực hiện hoạt động đại lý bảo hiểm theo quy định của pháp luật.
+C.  Người đại diện cho khách hàng.
+D. A, B, C đúng.</t>
+  </si>
+  <si>
+    <t>13. Mức vốn pháp định của doanh nghiệp bảo hiểm nhân thọ, kinh doanh bảo hiểm nhân thọ (bao gồm cả bảo hiểm liên kết đơn vị, bảo hiểm hưu trí) và bảo hiểm sức khỏe là:</t>
+  </si>
+  <si>
+    <t>A. 600 tỷ đồng Việt Nam
+B. 800 tỷ đồng Việt Nam
+C. 1.000 tỷ đồng Việt Nam
+D. 300 tỷ đồng Việt Nam</t>
+  </si>
+  <si>
+    <t>A. Thu xếp giải quyết bồi thường, trả tiền bảo hiểm khi xảy ra sự kiện bảo hiểm.
+B. Đánh giá rủi ro.
+C. Giới thiệu, chào bán bảo hiểm. 
+D. Thu phí bảo hiểm.</t>
+  </si>
+  <si>
+    <t>15. Theo quy định của Pháp luật, phát biểu nào dưới đây sai:</t>
+  </si>
+  <si>
+    <t>A. Các loại hợp đồng bảo hiểm bao gồm: hợp đồng bảo hiểm con người, hợp đồng bảo hiểm tài sản, hợp đồng bảo hiểm trách nhiệm dân sự.
+B. Hợp đồng bảo hiểm là sự thỏa thuận giữa bên mua bảo hiểm và doanh nghiệp bảo hiểm, theo đó bên mua bảo hiểm phải đóng phí bảo hiểm, doanh nghiệp bảo hiểm phải trả tiền bảo hiểm cho người thụ hưởng hoặc bồi thường cho người được bảo hiểm khi xảy ra sự kiện bảo hiểm.
+C. Hợp đồng bảo hiểm phải được lập thành văn bản.
+D. Trong trường hợp hợp đồng bảo hiểm có điều khoản không rõ ràng thì điều khoản đó được giải thích theo hướng có lợi cho doanh nghiệp bảo hiểm.</t>
+  </si>
+  <si>
+    <t>16. Đối với nghiệp vụ bảo hiểm trọn đời, doanh nghiệp bảo hiểm không có trách nhiệm đối với sự kiện nào sau đây:</t>
+  </si>
+  <si>
+    <t>A. Bên mua bảo hiểm chết vào bất kỳ thời điểm nào trong suốt cuộc đời của người đó (A)
+B. Người thụ hưởng chết vào bất kỳ thời điểm nào trong suốt cuộc đời của người đó (B)
+C. Người được bảo hiểm chết vào bất kỳ thời điểm nào trong suốt cuộc đời của người đó
+D. A, B đúng</t>
+  </si>
+  <si>
+    <t>17. Với Sản phẩm Bảo hiểm Ung Thư 360, khách hàng có những lựa chọn gói Bảo hiểm nào sau đây: </t>
+  </si>
+  <si>
+    <t>A. Một trong bốn gói với STBH tương ứng: 200 triệu, 400 triệu, 600 triệu và 800 triệu đồng. 
+B. Số tiền bảo hiểm tối đa 10 tỷ đồng. 
+C. Một trong bốn gói với STBH tương ứng: 500 triệu; 01 tỷ; 1,5 tỷ và 2 tỷ đồng. 
+D. Một trong bốn gói với STBH tương ứng: 300 triệu, 500 triệu, 700 triệu, 01 tỷ đồng; và gói tùy chọn với STBH tối thiểu 100 triệu đồng, tối đa 01 tỷ đồng. </t>
+  </si>
+  <si>
+    <t>18. Theo Luật kinh doanh bảo hiểm, ngoài các nghiệp vụ bảo hiểm đặc thù do Chính phủ qui định, các nghiệp vụ bảo hiểm được chia thành:</t>
+  </si>
+  <si>
+    <t>A. Bảo hiểm con người, bảo hiểm tài sản và bảo hiểm trách nhiệm dân sự.
+B. Bảo hiểm cá nhân, bảo hiểm nhóm.
+C. Bảo hiểm ngắn hạn, bảo hiểm dài hạn.
+D. Bảo hiểm nhân thọ, bảo hiểm phi nhân thọ và bảo hiểm sức khỏe. </t>
+  </si>
+  <si>
+    <t>19. Đáp án nào dưới đây đúng:</t>
+  </si>
+  <si>
+    <t>A. Đại lý bảo hiểm có thể lựa chọn và ký kết hợp đồng đại lý bảo hiểm với doanh nghiệp bảo hiểm, chi nhánh doanh nghiệp bảo hiểm phi nhân thọ nước ngoài
+B. Hoa hồng đại lý bảo hiểm được chi trả cho bên mua bảo hiểm và doanh nghiệp môi giới bảo hiểm
+C. Hoa hồng đại lý bảo hiểm được chi trả cho bên mua bảo hiểm và đại lý bảo hiểm
+D. Đại lý bảo hiểm có thể sửa đổi, bổ sung quy tắc, điều khoản bảo hiểm cho phù hợp với tình hình thực tế của khách hàng.</t>
+  </si>
+  <si>
+    <t>20. Theo quy định của Pháp luật, đáp án nào đúng khi nói về việc chuyển nhượng hợp đồng bảo hiểm:</t>
+  </si>
+  <si>
+    <t>A. Hợp đồng bảo hiểm không được chuyển nhượng
+B. Bên mua bảo hiểm có thể chuyển nhượng hợp đồng bảo hiểm theo thỏa thuận trong hợp đồng bảo hiểm
+C. Bên mua bảo hiểm có thể chuyển nhượng hợp đồng bảo hiểm cho bất kỳ người nào</t>
+  </si>
+  <si>
+    <t>21. Với Sản phẩm Bảo hiểm Ung Thư 360, số tiền bảo hiểm tối thiểu của một Hợp Đồng là: </t>
+  </si>
+  <si>
+    <t>A. 200 triệu đồng. 
+B. 250 triệu đồng. 
+C. 150 triệu đồng. 
+D. 100 triệu đồng. </t>
+  </si>
+  <si>
+    <t>22. Chọn phương án sai về khái niệm sau:</t>
+  </si>
+  <si>
+    <t>A. Người được bảo hiểm có thể đồng thời là người thụ hưởng
+B. Bên mua bảo hiểm có thể đồng thời là người được bảo hiểm và người thụ hưởng.
+C. Người thụ hưởng là người được doanh nghiệp bảo hiểm chỉ định để nhận tiền bảo hiểm theo hợp đồng bảo hiểm con người.   
+D. Người thụ hưởng là người được bên mua bảo hiểm chỉ định để nhận tiền bảo hiểm theo hợp đồng bảo hiểm con người.   </t>
+  </si>
+  <si>
+    <t>23. Theo Luật kinh doanh bảo hiểm, trường hợp doanh nghiệp bảo hiểm không phải bồi thường hoặc không phải trả tiền bảo hiểm khi xảy ra sự kiện bảo hiểm thì:</t>
+  </si>
+  <si>
+    <t>A. Phải được quy định rõ trong hợp đồng bảo hiểm và được doanh nghiệp bảo hiểm giải thích rõ cho bên mua bảo hiểm khi giao kết hợp đồng.
+B. Không cần quy định rõ trong hợp đồng bảo hiểm mà thực hiện theo các nguyên tắc chung mang tính nội bộ doanh nghiệp bảo hiểm.
+C. Không cần quy định rõ trong hợp đồng bảo hiểm vì pháp luật đã quy định rõ các trường hợp này.
+D. Không cần quy định rõ trong hợp đồng bảo hiểm và áp dụng theo thông lệ quốc tế.</t>
+  </si>
+  <si>
+    <t>24. Bên mua bảo hiểm có thể được giảm phí bảo hiểm khi mua bảo hiểm nhân thọ, bảo hiểm sức khỏe trong trường hợp:</t>
+  </si>
+  <si>
+    <t>A. Mua bảo hiểm trực tiếp từ doanh nghiệp bảo hiểm và doanh nghiệp bảo hiểm không phải chi trả hoa hồng bảo hiểm cho đại lý bảo hiểm hoặc doanh nghiệp môi giới bảo hiểm
+B. Mua bảo hiểm thông qua đại lý bảo hiểm 
+C. A, B đúng</t>
+  </si>
+  <si>
+    <t>25.  Quyền lợi bảo hiểm rủi ro của sản phẩm bảo hiểm hưu trí phải bao gồm tối thiểu các quyền lợi nào?</t>
+  </si>
+  <si>
+    <t>A. Quyền lợi trợ cấp mai táng, quyền lợi chăm sóc y tế, quyền lợi hỗ trợ nằm viện.
+B. Quyền lợi chăm sóc y tế.
+C. Quyền lợi trợ cấp mai táng, quyền lợi tử vong hoặc thương tật toàn bộ vĩnh viễn, quyền lợi bảo hiểm thất nghiệp.
+D. Quyền lợi trợ cấp mai táng, quyền lợi tử vong hoặc thương tật toàn bộ vĩnh viễn.</t>
+  </si>
+  <si>
+    <t>26. Chọn phương án đúng khi nói về đại lý bảo hiểm: </t>
+  </si>
+  <si>
+    <t>A. Đại lý bảo hiểm chịu sự kiểm tra giám sát của cơ quan nhà nước có thẩm quyền và thực hiện đầy đủ nghĩa vụ tài chính theo quy định của pháp luật (A).
+B. Đại lý bảo hiểm thực hiện hợp đồng bảo hiểm theo phạm vi được ủy quyền trong hợp đồng đại lý bảo hiểm (B).
+C. Đại lý bảo hiểm có thể đem phí bảo hiểm đi đầu tư và trả một phần lãi cho doanh nghiệp bảo hiểm (C).
+D. A,B đúng</t>
+  </si>
+  <si>
+    <t>27. Tỷ lệ hoa hồng tối đa tính trên phí bảo hiểm của hợp đồng bảo hiểm nhân thọ cá nhân thuộc nghiệp vụ bảo hiểm liên kết đơn vị, thời hạn từ 10 năm trở lên, phương thức nộp phí một lần là: </t>
+  </si>
+  <si>
+    <t>A. 5%
+B. 10%
+C. 7%
+D. 15%</t>
+  </si>
+  <si>
+    <t>28. Theo Luật kinh doanh bảo hiểm, bảo hiểm nhân thọ hỗn hợp là nghiệp vụ bảo hiểm kết hợp:</t>
+  </si>
+  <si>
+    <t>A. Bảo hiểm tử kỳ và bảo hiểm hưu trí. 
+B. Bảo hiểm trọn đời và bảo hiểm hưu trí. 
+C. Bảo hiểm sinh kỳ và bảo hiểm trọn đời. 
+D. Bảo hiểm sinh kỳ và bảo hiểm tử kỳ. </t>
+  </si>
+  <si>
+    <t>29. Đơn vị nào dưới đây được phép kinh doanh bảo hiểm sức khỏe?</t>
+  </si>
+  <si>
+    <t>A. Doanh nghiệp bảo hiểm Nhân thọ, doanh nghiệp bảo hiểm Phi Nhân thọ
+B. Văn phòng doanh nghiệp bảo hiểm nước ngoài tại Việt Nam
+C. Văn phòng doanh nghiệp môi giới bảo hiểm nước ngoài tại Việt Nam
+D. A, B, C đúng</t>
+  </si>
+  <si>
+    <t>30. Đại lý bảo hiểm có quyền:</t>
+  </si>
+  <si>
+    <t>A. Tiết lộ thông tin liên quan đến khách hàng
+B. Tạm ứng hoặc cho khách hàng vay tiền để đóng phí
+C. Dùng tiền hoa hồng để giảm phí hoặc khuyến mãi cho khách hàng
+D. Được hưởng hoa hồng đại lý</t>
+  </si>
+  <si>
+    <t>31. Doanh nghiệp bảo hiểm có nghĩa vụ:</t>
+  </si>
+  <si>
+    <t>A. Giải thích cho bên mua bảo hiểm về các điều kiện, điều khoản bảo hiểm; quyền, nghĩa vụ của bên mua bảo hiểm.
+B. Trả tiền bảo hiểm kịp thời cho người thụ hưởng hoặc bồi thường cho người được bảo hiểm khi xảy ra sự kiện bảo hiểm.
+C. Giải thích bằng văn bản lý do từ chối trả tiền bảo hiểm.
+D. A, B, C đúng.</t>
+  </si>
+  <si>
+    <t>32. Thông thường một hợp đồng bảo hiểm nhân thọ bị chấm dứt vì không tiếp tục đóng phí bảo hiểm, có thể khôi phục:</t>
+  </si>
+  <si>
+    <t>A. Trong vòng 2 năm kể từ khi mất hiệu lực và bên mua bảo hiểm đã đóng đủ phí bảo hiểm còn thiếu.
+B. Tại bất kỳ thời điểm nào kể từ khi mất hiệu lực và bên mua bảo hiểm đã đóng đủ phí bảo hiểm còn thiếu.  
+C. Trong vòng 4 năm kể từ khi mất hiệu lực và bên mua bảo hiểm đã đóng đủ phí bảo hiểm còn thiếu.
+D. Trong vòng 3 năm kể từ khi mất hiệu lực và bên mua bảo hiểm đã đóng đủ phí bảo hiểm còn thiếu.</t>
+  </si>
+  <si>
+    <t>33. Theo Pháp luật kinh doanh bảo hiểm, đối tượng nào sau đây có trách nhiệm nộp Quỹ bảo vệ người được bảo hiểm?</t>
+  </si>
+  <si>
+    <t>A. Doanh nghiệp bảo hiểm, chi nhánh doanh nghiệp bảo hiểm phi nhân thọ nước ngoài, doanh nghiệp môi giới bảo hiểm, đại lý bảo hiểm.
+B. Doanh nghiệp bảo hiểm, chi nhánh doanh nghiệp bảo hiểm phi nhân thọ nước ngoài (trừ doanh nghiệp bảo hiểm sức khỏe).
+C. Doanh nghiệp bảo hiểm, chi nhánh doanh nghiệp bảo hiểm phi nhân thọ nước ngoài, doanh nghiệp môi giới bảo hiểm.
+D. Doanh nghiệp bảo hiểm, chi nhánh doanh nghiệp bảo hiểm phi nhân thọ nước ngoài (trừ doanh nghiệp tái bảo hiểm).</t>
+  </si>
+  <si>
+    <t>34. Kể từ sau thời điểm Manulife đồng ý chi trả quyền lợi Ung Thư Giai Đoạn Cuối cho Người Được Bảo Hiểm của hợp đồng Bảo hiểm Ung Thư 360, vào mỗi ngày kỷ niệm hợp đồng hàng tháng, Manulife sẽ chi trả QLBH Trợ Cấp Thu Nhập bằng:</t>
+  </si>
+  <si>
+    <t>35. Hợp đồng bảo hiểm nhân thọ chấm dứt trong các trường hợp nào sau đây:</t>
+  </si>
+  <si>
+    <t>A. Bên mua bảo hiểm không còn quyền lợi có thể được bảo hiểm.
+B. Bên mua bảo hiểm tham gia một hợp đồng bảo hiểm khác cung cấp quyền lợi tương tự
+C. Câu A và B đều đúng
+D. Câu A và B đều sai</t>
+  </si>
+  <si>
+    <t>36. Trong Sản phẩm Bảo hiểm Ung Thư 360, thời hạn tối đa để con của Người Được Bảo Hiểm hoặc người giám hộ hợp pháp của con của Người Được Bảo Hiểm gửi yêu cầu và hoàn thành hồ sơ yêu cầu Manulife cấp quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của NĐBH là:</t>
+  </si>
+  <si>
+    <t>A. 07 ngày kể từ ngày  Manulife chấp nhận chi trả Quyền lợi Ung Thư Giai Đoạn Cuối.
+B. 60 ngày kể từ ngày Manulife chấp nhận chi trả Quyền lợi Ung Thư Giai Đoạn Cuối.
+C. 90 ngày kể từ ngày Manulife chấp nhận chi trả Quyền lợi Ung Thư Giai Đoạn Cuối.
+D. 30 ngày kể từ ngày  Manulife chấp nhận chi trả Quyền lợi Ung Thư Giai Đoạn Cuối.</t>
+  </si>
+  <si>
+    <t>37. Theo Luật kinh doanh bảo hiểm, kinh doanh bảo hiểm là:</t>
+  </si>
+  <si>
+    <t>A. Hoạt động của doanh nghiệp bảo hiểm nhằm mục đích sinh lợi, theo đó doanh nghiệp bảo hiểm chấp nhận rủi ro của người được bảo hiểm, trên cơ sở bên mua bảo hiểm đóng phí bảo hiểm để doanh nghiệp bảo hiểm trả tiền bảo hiểm cho người thụ hưởng hoặc bồi thường cho người được bảo hiểm khi xảy ra sự kiện bảo hiểm.
+B. Hoạt động của doanh nghiệp bảo hiểm nhằm mục đích sinh lợi, theo đó doanh nghiệp bảo hiểm nhận một khoản phí bảo hiểm của doanh nghiệp bảo hiểm khác để cam kết bồi thường cho các trách nhiệm đã nhận bảo hiểm.
+C. Cả A và B</t>
+  </si>
+  <si>
+    <t>38. Chọn phương án sai về đại lý bảo hiểm:</t>
+  </si>
+  <si>
+    <t>A. Đại lý bảo hiểm được hưởng hoa hồng bảo hiểm do doanh nghiệp bảo hiểm trả.
+B. Đại lý bảo hiểm là người đại diện cho khách hàng tham gia bảo hiểm.
+C. Đại lý bảo hiểm có thể được doanh nghiệp bảo hiểm ủy quyền trả tiền bảo hiểm.
+D. Đại lý bảo hiểm là người được doanh nghiệp bảo hiểm ủy quyền để thực hiện những công việc liên quan đến hợp đồng bảo hiểm.</t>
+  </si>
+  <si>
+    <t>39. Đối với hợp đồng bảo hiểm con người, trường hợp một hoặc một số người thụ hưởng cố ý gây ra cái chết hoặc thương tật vĩnh viễn cho người được bảo hiểm thì:</t>
+  </si>
+  <si>
+    <t>40. Trong Sản phẩm Bảo hiểm Ung Thư 360, trong trường hợp con của Người Được Bảo Hiểm được Manulife chấp thuận cấp quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của Người Được Bảo Hiểm, ngày bắt đầu bảo hiểm sẽ là:</t>
+  </si>
+  <si>
+    <t>A. Ngày Manulife đồng ý cấp quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của Người Được Bảo Hiểm
+B. Ngày Người Được Bảo Hiểm được chẩn đoán mắc bệnh Ung Thư Giai Đoạn Cuối
+C. Ngày hoàn thành hồ sơ yêu cầu cấp quyền lợi Bảo Hiểm Miễn Phí Dành Cho Con Của Người Được Bảo Hiểm
+D. Ngày Manulife chấp nhận chi trả quyền lợi Ung Thư Giai Đoạn Cuối cho Người Được Bảo Hiểm.</t>
   </si>
 </sst>
 </file>
@@ -1561,10 +2288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="K142" sqref="K142"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1575,2010 +2302,3164 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s" s="0">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s" s="0">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s" s="0">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s" s="0">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s" s="0">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s" s="0">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s" s="0">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s" s="0">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s" s="0">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s" s="0">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s" s="0">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s" s="0">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s" s="0">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s" s="0">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s" s="0">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s" s="0">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s" s="0">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s" s="0">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s" s="0">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s" s="0">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s" s="0">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s" s="0">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s" s="0">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s" s="0">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s" s="0">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s" s="0">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s" s="0">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s" s="0">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s" s="0">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s" s="0">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s" s="0">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s" s="0">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s" s="0">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s" s="0">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s" s="0">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s" s="0">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s" s="0">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s" s="0">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s" s="0">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s" s="0">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s" s="0">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s" s="0">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s" s="0">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s" s="0">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s" s="0">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s" s="0">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s" s="0">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D74" t="s" s="0">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s" s="0">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s" s="0">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D76" t="s" s="0">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s" s="0">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D77" t="s" s="0">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s" s="0">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s" s="0">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D79" t="s" s="0">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s" s="0">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D80" t="s" s="0">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s" s="0">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D81" t="s" s="0">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s" s="0">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B82" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D82" t="s" s="0">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s" s="0">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B83" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D83" t="s" s="0">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s" s="0">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D84" t="s" s="0">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s" s="0">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B85" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D85" t="s" s="0">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s" s="0">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B86" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D86" t="s" s="0">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s" s="0">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D87" t="s" s="0">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s" s="0">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D88" t="s" s="0">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s" s="0">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D89" t="s" s="0">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s" s="0">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D90" t="s" s="0">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s" s="0">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D91" t="s" s="0">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s" s="0">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D92" t="s" s="0">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s" s="0">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D93" t="s" s="0">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s" s="0">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D94" t="s" s="0">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s" s="0">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D95" t="s" s="0">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s" s="0">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D96" t="s" s="0">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s" s="0">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s" s="0">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C98" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s" s="0">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C99" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s" s="0">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D100" t="s" s="0">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s" s="0">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D101" t="s" s="0">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s" s="0">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C102" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D102" t="s" s="0">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s" s="0">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C103" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D103" t="s" s="0">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s" s="0">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D104" t="s" s="0">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s" s="0">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B105" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D105" t="s" s="0">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s" s="0">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C106" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D106" t="s" s="0">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s" s="0">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B107" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C107" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D107" t="s" s="0">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s" s="0">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B108" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C108" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D108" t="s" s="0">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s" s="0">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B109" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D109" t="s" s="0">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s" s="0">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B110" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C110" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D110" t="s" s="0">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s" s="0">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B111" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D111" t="s" s="0">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s" s="0">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B112" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C112" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D112" t="s" s="0">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s" s="0">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B113" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C113" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D113" t="s" s="0">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s" s="0">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B114" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C114" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D114" t="s" s="0">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s" s="0">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B115" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C115" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D115" t="s" s="0">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s" s="0">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B116" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C116" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D116" t="s" s="0">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s" s="0">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B117" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C117" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D117" t="s" s="0">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s" s="0">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B118" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C118" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D118" t="s" s="0">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s" s="0">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B119" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C119" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D119" t="s" s="0">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s" s="0">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B120" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C120" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D120" t="s" s="0">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s" s="0">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B121" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C121" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D121" t="s" s="0">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s" s="0">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B122" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C122" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D122" t="s" s="0">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s" s="0">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B123" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C123" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D123" t="s" s="0">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s" s="0">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B124" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C124" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D124" t="s" s="0">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s" s="0">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B125" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C125" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D125" t="s" s="0">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s" s="0">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B126" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C126" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D126" t="s" s="0">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s" s="0">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B127" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C127" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D127" t="s" s="0">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s" s="0">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B128" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C128" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D128" t="s" s="0">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s" s="0">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B129" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C129" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D129" t="s" s="0">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s" s="0">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B130" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C130" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D130" t="s" s="0">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s" s="0">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B131" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C131" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D131" t="s" s="0">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s" s="0">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B132" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C132" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D132" t="s" s="0">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s" s="0">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B133" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C133" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D133" t="s" s="0">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s" s="0">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B134" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C134" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D134" t="s" s="0">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s" s="0">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B135" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C135" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D135" t="s" s="0">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s" s="0">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B136" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C136" t="s" s="0">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D136" t="s" s="0">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s" s="0">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B137" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C137" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D137" t="s" s="0">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s" s="0">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B138" t="s" s="0">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C138" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D138" t="s" s="0">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s" s="0">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B139" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C139" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D139" t="s" s="0">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s" s="0">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B140" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C140" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D140" t="s" s="0">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s" s="0">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B141" t="s" s="0">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C141" t="s" s="0">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D141" t="s" s="0">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s" s="0">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B142" t="s" s="0">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C142" t="s" s="0">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D142" t="s" s="0">
+        <v>283</v>
+      </c>
+      <c r="E142" t="s" s="0">
         <v>287</v>
-      </c>
-      <c r="E142" t="s" s="0">
-        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s" s="0">
+        <v>284</v>
+      </c>
+      <c r="B143" t="s" s="0">
+        <v>281</v>
+      </c>
+      <c r="C143" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D143" t="s" s="0">
+        <v>285</v>
+      </c>
+      <c r="E143" t="s" s="0">
         <v>288</v>
       </c>
-      <c r="B143" t="s" s="0">
-        <v>285</v>
-      </c>
-      <c r="C143" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D143" t="s" s="0">
-        <v>289</v>
+    </row>
+    <row r="144" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A144" t="s" s="0">
+        <v>292</v>
+      </c>
+      <c r="B144" t="s" s="0">
+        <v>281</v>
+      </c>
+      <c r="C144" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E144" t="s" s="0">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A145" t="s" s="0">
+        <v>296</v>
+      </c>
+      <c r="B145" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C145" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="0">
+        <v>299</v>
+      </c>
+      <c r="B146" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C146" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D146" t="s" s="0">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="0">
+        <v>301</v>
+      </c>
+      <c r="B147" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C147" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D147" t="s" s="0">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="0">
+        <v>303</v>
+      </c>
+      <c r="B148" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C148" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D148" t="s" s="0">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="0">
+        <v>305</v>
+      </c>
+      <c r="B149" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C149" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D149" t="s" s="0">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="0">
+        <v>307</v>
+      </c>
+      <c r="B150" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C150" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D150" t="s" s="0">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="0">
+        <v>309</v>
+      </c>
+      <c r="B151" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C151" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D151" t="s" s="0">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="0">
+        <v>311</v>
+      </c>
+      <c r="B152" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C152" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D152" t="s" s="0">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="B153" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C153" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D153" t="s" s="0">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="0">
+        <v>315</v>
+      </c>
+      <c r="B154" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C154" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D154" t="s" s="0">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="0">
+        <v>317</v>
+      </c>
+      <c r="B155" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C155" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D155" t="s" s="0">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="B156" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C156" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D156" t="s" s="0">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="0">
+        <v>321</v>
+      </c>
+      <c r="B157" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C157" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D157" t="s" s="0">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="0">
+        <v>323</v>
+      </c>
+      <c r="B158" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C158" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D158" t="s" s="0">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="B159" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C159" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D159" t="s" s="0">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="0">
+        <v>327</v>
+      </c>
+      <c r="B160" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C160" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D160" t="s" s="0">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s" s="0">
+        <v>329</v>
+      </c>
+      <c r="B161" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C161" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D161" t="s" s="0">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="0">
+        <v>331</v>
+      </c>
+      <c r="B162" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C162" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D162" t="s" s="0">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="0">
+        <v>333</v>
+      </c>
+      <c r="B163" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C163" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D163" t="s" s="0">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s" s="0">
+        <v>335</v>
+      </c>
+      <c r="B164" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C164" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D164" t="s" s="0">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s" s="0">
+        <v>337</v>
+      </c>
+      <c r="B165" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C165" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D165" t="s" s="0">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="0">
+        <v>339</v>
+      </c>
+      <c r="B166" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C166" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D166" t="s" s="0">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="B167" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C167" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D167" t="s" s="0">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B168" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C168" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D168" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B169" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C169" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D169" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B170" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C170" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D170" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B171" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C171" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D171" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B172" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C172" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D172" t="s" s="0">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s" s="0">
+        <v>353</v>
+      </c>
+      <c r="B173" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C173" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D173" t="s" s="0">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s" s="0">
+        <v>355</v>
+      </c>
+      <c r="B174" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C174" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D174" t="s" s="0">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s" s="0">
+        <v>357</v>
+      </c>
+      <c r="B175" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C175" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D175" t="s" s="0">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s" s="0">
+        <v>359</v>
+      </c>
+      <c r="B176" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C176" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D176" t="s" s="0">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s" s="0">
+        <v>361</v>
+      </c>
+      <c r="B177" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C177" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D177" t="s" s="0">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s" s="0">
+        <v>363</v>
+      </c>
+      <c r="B178" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C178" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D178" t="s" s="0">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s" s="0">
+        <v>365</v>
+      </c>
+      <c r="B179" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C179" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D179" t="s" s="0">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s" s="0">
+        <v>367</v>
+      </c>
+      <c r="B180" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C180" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D180" t="s" s="0">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s" s="0">
+        <v>369</v>
+      </c>
+      <c r="B181" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C181" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D181" t="s" s="0">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s" s="0">
+        <v>371</v>
+      </c>
+      <c r="B182" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C182" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D182" t="s" s="0">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="B183" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C183" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D183" t="s" s="0">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B184" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C184" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D184" t="s" s="0">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s" s="0">
+        <v>377</v>
+      </c>
+      <c r="B185" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C185" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D185" t="s" s="0">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s" s="0">
+        <v>379</v>
+      </c>
+      <c r="B186" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C186" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D186" t="s" s="0">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s" s="0">
+        <v>381</v>
+      </c>
+      <c r="B187" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C187" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D187" t="s" s="0">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s" s="0">
+        <v>383</v>
+      </c>
+      <c r="B188" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C188" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D188" t="s" s="0">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s" s="0">
+        <v>385</v>
+      </c>
+      <c r="B189" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C189" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D189" t="s" s="0">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s" s="0">
+        <v>387</v>
+      </c>
+      <c r="B190" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C190" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D190" t="s" s="0">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s" s="0">
+        <v>389</v>
+      </c>
+      <c r="B191" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C191" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D191" t="s" s="0">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s" s="0">
+        <v>391</v>
+      </c>
+      <c r="B192" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C192" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D192" t="s" s="0">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s" s="0">
+        <v>393</v>
+      </c>
+      <c r="B193" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C193" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D193" t="s" s="0">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s" s="0">
+        <v>395</v>
+      </c>
+      <c r="B194" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C194" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D194" t="s" s="0">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s" s="0">
+        <v>397</v>
+      </c>
+      <c r="B195" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C195" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D195" t="s" s="0">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s" s="0">
+        <v>399</v>
+      </c>
+      <c r="B196" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C196" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D196" t="s" s="0">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s" s="0">
+        <v>401</v>
+      </c>
+      <c r="B197" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C197" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D197" t="s" s="0">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s" s="0">
+        <v>403</v>
+      </c>
+      <c r="B198" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C198" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D198" t="s" s="0">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="B199" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C199" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D199" t="s" s="0">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s" s="0">
+        <v>406</v>
+      </c>
+      <c r="B200" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C200" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D200" t="s" s="0">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s" s="0">
+        <v>408</v>
+      </c>
+      <c r="B201" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C201" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D201" t="s" s="0">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s" s="0">
+        <v>410</v>
+      </c>
+      <c r="B202" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C202" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D202" t="s" s="0">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s" s="0">
+        <v>412</v>
+      </c>
+      <c r="B203" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C203" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D203" t="s" s="0">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s" s="0">
+        <v>414</v>
+      </c>
+      <c r="B204" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C204" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D204" t="s" s="0">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s" s="0">
+        <v>416</v>
+      </c>
+      <c r="B205" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C205" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D205" t="s" s="0">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s" s="0">
+        <v>418</v>
+      </c>
+      <c r="B206" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C206" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D206" t="s" s="0">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s" s="0">
+        <v>420</v>
+      </c>
+      <c r="B207" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C207" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D207" t="s" s="0">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s" s="0">
+        <v>422</v>
+      </c>
+      <c r="B208" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C208" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D208" t="s" s="0">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s" s="0">
+        <v>424</v>
+      </c>
+      <c r="B209" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C209" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D209" t="s" s="0">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s" s="0">
+        <v>426</v>
+      </c>
+      <c r="B210" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C210" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D210" t="s" s="0">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s" s="0">
+        <v>428</v>
+      </c>
+      <c r="B211" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C211" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D211" t="s" s="0">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s" s="0">
+        <v>430</v>
+      </c>
+      <c r="B212" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C212" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D212" t="s" s="0">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s" s="0">
+        <v>432</v>
+      </c>
+      <c r="B213" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C213" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D213" t="s" s="0">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s" s="0">
+        <v>434</v>
+      </c>
+      <c r="B214" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C214" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D214" t="s" s="0">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s" s="0">
+        <v>436</v>
+      </c>
+      <c r="B215" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C215" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D215" t="s" s="0">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s" s="0">
+        <v>438</v>
+      </c>
+      <c r="B216" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C216" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D216" t="s" s="0">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s" s="0">
+        <v>440</v>
+      </c>
+      <c r="B217" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C217" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D217" t="s" s="0">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s" s="0">
+        <v>442</v>
+      </c>
+      <c r="B218" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C218" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D218" t="s" s="0">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s" s="0">
+        <v>444</v>
+      </c>
+      <c r="B219" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C219" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D219" t="s" s="0">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s" s="0">
+        <v>445</v>
+      </c>
+      <c r="B220" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C220" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D220" t="s" s="0">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s" s="0">
+        <v>447</v>
+      </c>
+      <c r="B221" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C221" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D221" t="s" s="0">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s" s="0">
+        <v>449</v>
+      </c>
+      <c r="B222" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C222" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D222" t="s" s="0">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s" s="0">
+        <v>451</v>
+      </c>
+      <c r="B223" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C223" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D223" t="s" s="0">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s" s="0">
+        <v>453</v>
+      </c>
+      <c r="B224" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C224" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D224" t="s" s="0">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s" s="0">
+        <v>454</v>
+      </c>
+      <c r="B225" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="C225" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D225" t="s" s="0">
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -3588,7 +5469,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7375D0D9-A088-4E33-84C0-F60360358F66}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -3601,15 +5482,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B1" s="0">
-        <v>165</v>
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>272.0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -3617,23 +5498,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0">
         <v>0</v>
@@ -3641,7 +5522,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0">
         <v>30</v>
@@ -3649,7 +5530,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0">
         <v>0</v>
@@ -3657,7 +5538,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0">
         <v>0</v>
@@ -3665,7 +5546,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="0">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0">
         <v>0</v>
@@ -3673,7 +5554,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0">
         <v>0</v>
@@ -3681,7 +5562,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s" s="0">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0">
         <v>0</v>
@@ -3689,7 +5570,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s" s="0">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0">
         <v>0</v>
@@ -3697,7 +5578,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s" s="0">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0">
         <v>77</v>
@@ -3705,7 +5586,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0">
         <v>45</v>
@@ -3713,7 +5594,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0">
         <v>32</v>
@@ -3721,7 +5602,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s" s="0">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0">
         <v>0</v>
@@ -3729,15 +5610,15 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0">
         <v>0</v>
@@ -3745,7 +5626,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s" s="0">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0">
         <v>0</v>
@@ -3753,7 +5634,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20" s="0">
         <v>0</v>
@@ -3761,7 +5642,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s" s="0">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21" s="0">
         <v>1</v>
@@ -3769,7 +5650,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s" s="0">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B22" s="0">
         <v>2</v>
@@ -3777,10 +5658,18 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s" s="0">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B23" s="0">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s" s="0">
+        <v>298</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>105.0</v>
       </c>
     </row>
   </sheetData>
@@ -3790,10 +5679,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E57CE46-9D74-4C06-8F20-8319158C49B7}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3818,47 +5707,70 @@
         <v>2700</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F1" t="s" s="0">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>3</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>4</v>
+        <v>278</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>5</v>
+        <v>279</v>
       </c>
       <c r="D2" s="0">
-        <v>5400</v>
+        <v>600</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>6</v>
+        <v>286</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D3" s="0">
         <v>600</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
         <v>290</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>279</v>
+      <c r="B4" t="s" s="0">
+        <v>278</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>278</v>
+      </c>
+      <c r="D4" s="0">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>291</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix everything 4 (final)
</commit_message>
<xml_diff>
--- a/src/main/java/data/QuizTestAppData.xlsx
+++ b/src/main/java/data/QuizTestAppData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="509">
   <si>
     <t>root</t>
   </si>
@@ -1923,6 +1923,257 @@
   </si>
   <si>
     <t>,171,202</t>
+  </si>
+  <si>
+    <t>Thành phố nào là thủ đô của Brazil?</t>
+  </si>
+  <si>
+    <t>A. Brasília
+B. Rio de Janeiro
+C. São Paulo</t>
+  </si>
+  <si>
+    <t>Dòng sông nổi tiếng chảy qua thung lũng lịch sử nổi tiếng Mesopotamia là:</t>
+  </si>
+  <si>
+    <t>A. Sông Amazon
+B. Sông Nile
+C. Sông Eufrat</t>
+  </si>
+  <si>
+    <t>Đồng bằng nổi tiếng và phù hợp cho nông nghiệp nằm ở miền Bắc Việt Nam là:</t>
+  </si>
+  <si>
+    <t>A. Đồng bằng Sông Cửu Long
+B. Đồng bằng Sông Hồng
+C. Đồng bằng Sông Mê Kông</t>
+  </si>
+  <si>
+    <t>Quốc gia nào không nằm ở châu Á?</t>
+  </si>
+  <si>
+    <t>A. Nhật Bản
+B. Ấn Độ
+C. Brazil</t>
+  </si>
+  <si>
+    <t>Thành phố lớn nhất nước Mỹ là:</t>
+  </si>
+  <si>
+    <t>A. New York
+B. Los Angeles
+C. Chicago</t>
+  </si>
+  <si>
+    <t>Quốc gia nằm ở Đông Nam Á, có thủ đô là Jakarta là:</t>
+  </si>
+  <si>
+    <t>A. Indonesia
+B. Malaysia
+C. Philippines</t>
+  </si>
+  <si>
+    <t>Đỉnh núi nổi tiếng ở châu Phi là:</t>
+  </si>
+  <si>
+    <t>A. Everest
+B. Kilimanjaro
+C. Mont Blanc</t>
+  </si>
+  <si>
+    <t>Quốc gia nào nằm ở Bán đảo Iberia?</t>
+  </si>
+  <si>
+    <t>A. Tây Ban Nha
+B. Italia
+C. Hy Lạp</t>
+  </si>
+  <si>
+    <t>Đảo nổi tiếng với tượng chúa Kitô Vua là:</t>
+  </si>
+  <si>
+    <t>A. Đảo Hawaii
+B. Đảo Jeju
+C. Đảo Corcovado</t>
+  </si>
+  <si>
+    <t>Thành phố nổi tiếng với Cung điện Buckingham là:</t>
+  </si>
+  <si>
+    <t>A. Paris
+B. London
+C. Moscow</t>
+  </si>
+  <si>
+    <t>Quốc gia nào có dân số đông nhất thế giới?</t>
+  </si>
+  <si>
+    <t>A. Trung Quốc
+B. Ấn Độ
+C. Mỹ</t>
+  </si>
+  <si>
+    <t>Dòng sông Mississippi chảy qua bao nhiêu bang của Mỹ?</t>
+  </si>
+  <si>
+    <t>A. 1
+B. 2
+C. 3</t>
+  </si>
+  <si>
+    <t>Thành phố nào là thủ đô của Ý?</t>
+  </si>
+  <si>
+    <t>A. Roma
+B. Milano
+C. Napoli</t>
+  </si>
+  <si>
+    <t>Đảo nằm giữa biển Địa Trung Hải và được biết đến với cung điện Alhambra là:</t>
+  </si>
+  <si>
+    <t>A. Đảo Balearic
+B. Đảo Corsica
+C. Đảo Sicily</t>
+  </si>
+  <si>
+    <t>Hệ thống đường sắt lớn nhất châu Âu là:</t>
+  </si>
+  <si>
+    <t>A. Eurostar
+B. TGV
+C. Trans-Siberian</t>
+  </si>
+  <si>
+    <t>Quốc gia nào là quê hương của đền Taj Mahal?</t>
+  </si>
+  <si>
+    <t>A. Ấn Độ
+B. Trung Quốc
+C. Nhật Bản</t>
+  </si>
+  <si>
+    <t>Dải đất hẹp nằm giữa biển Đen và biển Địa Trung Hải là:</t>
+  </si>
+  <si>
+    <t>A. Bán đảo Balkan
+B. Bán đảo Iberia
+C. Bán đảo Scandinavia</t>
+  </si>
+  <si>
+    <t>Núi lửa Vesuvius nằm ở quốc gia nào?</t>
+  </si>
+  <si>
+    <t>A. Ý
+B. Tây Ban Nha
+C. Hy Lạp</t>
+  </si>
+  <si>
+    <t>Quốc gia nào là quê hương của vịnh Hạ Long?</t>
+  </si>
+  <si>
+    <t>A. Việt Nam
+B. Thái Lan
+C. Indonesia</t>
+  </si>
+  <si>
+    <t>Dải đất hẹp nằm giữa biển Caribe và Đại Tây Dương là:</t>
+  </si>
+  <si>
+    <t>A. Bán đảo Florida
+B. Bán đảo Yucatan
+C. Bán đảo Labrador</t>
+  </si>
+  <si>
+    <t>Thành phố nào được gọi là "thành phố không bao giờ ngủ"?</t>
+  </si>
+  <si>
+    <t>A. Tokyo
+B. New York
+C. London</t>
+  </si>
+  <si>
+    <t>Đồng bằng lớn nhất thế giới là:</t>
+  </si>
+  <si>
+    <t>A. Đồng bằng Sông Cửu Long
+B. Đồng bằng Ganges-Brahmaputra
+C. Đồng bằng Amazon</t>
+  </si>
+  <si>
+    <t>Quốc gia nào là quê hương của vùng đất tuyết Alaska?</t>
+  </si>
+  <si>
+    <t>A. Canada
+B. Mỹ
+C. Nga</t>
+  </si>
+  <si>
+    <t>Đảo nổi tiếng với khối núi Phật A Di Đà là:</t>
+  </si>
+  <si>
+    <t>A. Đảo Bali
+B. Đảo Lombok
+C. Đảo Jeju</t>
+  </si>
+  <si>
+    <t>Dòng sông nào là dòng sông dài nhất châu Á?</t>
+  </si>
+  <si>
+    <t>A. Sông Mekong
+B. Sông Ganges
+C. Sông Yangtze</t>
+  </si>
+  <si>
+    <t>Quốc gia nào nằm ở Bắc Âu?</t>
+  </si>
+  <si>
+    <t>A. Phần Lan
+B. Hà Lan
+C. Đan Mạch</t>
+  </si>
+  <si>
+    <t>Quốc gia nào nằm ở khu vực Đông Nam Á?</t>
+  </si>
+  <si>
+    <t>A. Argentina
+B. Malaysia
+C. Ba Lan</t>
+  </si>
+  <si>
+    <t>Đại ngàn nổi tiếng của Việt Nam là:</t>
+  </si>
+  <si>
+    <t>A. Đại Sơn
+B. Trường Sơn
+C. Trường Giang</t>
+  </si>
+  <si>
+    <t>Nước nào là quốc gia lớn nhất thế giới về diện tích?</t>
+  </si>
+  <si>
+    <t>A. Nga
+B. Trung Quốc
+C. Mỹ</t>
+  </si>
+  <si>
+    <t>Kênh đào nổi tiếng nằm ở Ai Cập là:</t>
+  </si>
+  <si>
+    <t>A. Kênh Panama
+B. Kênh Suez
+C. Kênh Kiel</t>
+  </si>
+  <si>
+    <t>A. In here
+B. In some where
+C. Ở đâu đó</t>
+  </si>
+  <si>
+    <t>,171,202,170</t>
+  </si>
+  <si>
+    <t>A, B, C</t>
   </si>
 </sst>
 </file>
@@ -2241,7 +2492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E203"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
     <sheetView topLeftCell="A163" workbookViewId="0">
       <selection activeCell="C171" sqref="C171"/>
@@ -4659,10 +4910,13 @@
         <v>21</v>
       </c>
       <c r="C171" t="s" s="0">
-        <v>24</v>
+        <v>508</v>
       </c>
       <c r="D171" t="s" s="0">
-        <v>377</v>
+        <v>506</v>
+      </c>
+      <c r="E171" t="s" s="0">
+        <v>203</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
@@ -5111,6 +5365,426 @@
       </c>
       <c r="D203" t="s" s="0">
         <v>444</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s" s="0">
+        <v>446</v>
+      </c>
+      <c r="B204" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C204" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D204" t="s" s="0">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s" s="0">
+        <v>448</v>
+      </c>
+      <c r="B205" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C205" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D205" t="s" s="0">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s" s="0">
+        <v>450</v>
+      </c>
+      <c r="B206" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C206" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D206" t="s" s="0">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s" s="0">
+        <v>452</v>
+      </c>
+      <c r="B207" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C207" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D207" t="s" s="0">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s" s="0">
+        <v>454</v>
+      </c>
+      <c r="B208" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C208" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D208" t="s" s="0">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s" s="0">
+        <v>456</v>
+      </c>
+      <c r="B209" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C209" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D209" t="s" s="0">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="B210" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C210" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D210" t="s" s="0">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s" s="0">
+        <v>460</v>
+      </c>
+      <c r="B211" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C211" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D211" t="s" s="0">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s" s="0">
+        <v>462</v>
+      </c>
+      <c r="B212" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C212" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D212" t="s" s="0">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s" s="0">
+        <v>464</v>
+      </c>
+      <c r="B213" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C213" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D213" t="s" s="0">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s" s="0">
+        <v>466</v>
+      </c>
+      <c r="B214" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C214" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D214" t="s" s="0">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s" s="0">
+        <v>468</v>
+      </c>
+      <c r="B215" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C215" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D215" t="s" s="0">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s" s="0">
+        <v>470</v>
+      </c>
+      <c r="B216" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C216" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D216" t="s" s="0">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s" s="0">
+        <v>472</v>
+      </c>
+      <c r="B217" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C217" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D217" t="s" s="0">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s" s="0">
+        <v>474</v>
+      </c>
+      <c r="B218" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C218" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D218" t="s" s="0">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s" s="0">
+        <v>476</v>
+      </c>
+      <c r="B219" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C219" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D219" t="s" s="0">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s" s="0">
+        <v>478</v>
+      </c>
+      <c r="B220" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C220" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D220" t="s" s="0">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s" s="0">
+        <v>480</v>
+      </c>
+      <c r="B221" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C221" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D221" t="s" s="0">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s" s="0">
+        <v>482</v>
+      </c>
+      <c r="B222" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C222" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D222" t="s" s="0">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s" s="0">
+        <v>484</v>
+      </c>
+      <c r="B223" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C223" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D223" t="s" s="0">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s" s="0">
+        <v>486</v>
+      </c>
+      <c r="B224" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C224" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D224" t="s" s="0">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s" s="0">
+        <v>488</v>
+      </c>
+      <c r="B225" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C225" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D225" t="s" s="0">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s" s="0">
+        <v>490</v>
+      </c>
+      <c r="B226" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C226" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D226" t="s" s="0">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s" s="0">
+        <v>492</v>
+      </c>
+      <c r="B227" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C227" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D227" t="s" s="0">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s" s="0">
+        <v>494</v>
+      </c>
+      <c r="B228" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C228" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D228" t="s" s="0">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s" s="0">
+        <v>496</v>
+      </c>
+      <c r="B229" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C229" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D229" t="s" s="0">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s" s="0">
+        <v>498</v>
+      </c>
+      <c r="B230" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C230" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D230" t="s" s="0">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s" s="0">
+        <v>500</v>
+      </c>
+      <c r="B231" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C231" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D231" t="s" s="0">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s" s="0">
+        <v>502</v>
+      </c>
+      <c r="B232" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C232" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D232" t="s" s="0">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s" s="0">
+        <v>504</v>
+      </c>
+      <c r="B233" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C233" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D233" t="s" s="0">
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -5137,7 +5811,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="n">
-        <v>203.0</v>
+        <v>233.0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -5232,8 +5906,8 @@
       <c r="A13" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B13" s="0">
-        <v>25</v>
+      <c r="B13" s="0" t="n">
+        <v>55.0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -5248,8 +5922,8 @@
       <c r="A15" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B15" s="0">
-        <v>0</v>
+      <c r="B15" s="0" t="n">
+        <v>30.0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -5495,7 +6169,7 @@
         <v>300</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>445</v>
+        <v>507</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>76</v>

</xml_diff>